<commit_message>
funzionante sicuramente fino al replace dei canali
</commit_message>
<xml_diff>
--- a/test_conv1d/test_conv1d/mem.xlsx
+++ b/test_conv1d/test_conv1d/mem.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="Questa_cartella_di_lavoro" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Titania\Desktop\ms\lab3\test_conv1d\test_conv1d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D67849C-A139-4C47-9044-14DDCBF20EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80859B24-E829-40A6-BC36-C2AC17E626FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12495" yWindow="0" windowWidth="7995" windowHeight="10920" xr2:uid="{0D9A6957-12B8-4496-A02D-3AD1E515C0C0}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="12960" windowHeight="9690" xr2:uid="{0D9A6957-12B8-4496-A02D-3AD1E515C0C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -605,10 +605,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C0074E-DEC8-4308-8A72-531CDC045EBC}">
+  <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:S128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -618,16 +619,16 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1">
-        <v>146</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="C1" s="1">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="D1" s="2">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E1" s="23" t="s">
         <v>0</v>
@@ -635,31 +636,31 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="3">
-        <v>198</v>
+        <v>83</v>
       </c>
       <c r="B2" s="4">
-        <v>101</v>
+        <v>217</v>
       </c>
       <c r="C2" s="3">
-        <v>108</v>
+        <v>251</v>
       </c>
       <c r="D2" s="4">
-        <v>254</v>
+        <v>10</v>
       </c>
       <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="3">
-        <v>179</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="C3" s="3">
-        <v>236</v>
+        <v>107</v>
       </c>
       <c r="D3" s="4">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E3" s="23"/>
       <c r="O3" s="21"/>
@@ -672,16 +673,16 @@
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="3">
-        <v>142</v>
+        <v>32</v>
       </c>
       <c r="B4" s="4">
-        <v>221</v>
+        <v>101</v>
       </c>
       <c r="C4" s="3">
-        <v>160</v>
+        <v>91</v>
       </c>
       <c r="D4" s="4">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="E4" s="23"/>
       <c r="O4" s="21" t="s">
@@ -702,16 +703,16 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="5">
-        <v>209</v>
+        <v>243</v>
       </c>
       <c r="B5" s="6">
-        <v>184</v>
+        <v>78</v>
       </c>
       <c r="C5" s="5">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="D5" s="6">
-        <v>1</v>
+        <v>131</v>
       </c>
       <c r="E5" s="23"/>
       <c r="O5" s="21">
@@ -719,27 +720,27 @@
       </c>
       <c r="P5" s="21">
         <f>SUM(out_col0!A1:D20)</f>
-        <v>1388393</v>
+        <v>1156924</v>
       </c>
       <c r="Q5">
         <f>SUM(out_col1!A1:D20)</f>
-        <v>1405895</v>
+        <v>1202454</v>
       </c>
       <c r="R5" s="21"/>
       <c r="S5" s="21"/>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="2">
-        <v>191</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1">
-        <v>80</v>
+        <v>255</v>
       </c>
       <c r="C6" s="2">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="E6" s="23"/>
       <c r="O6" s="21">
@@ -747,7 +748,7 @@
       </c>
       <c r="P6" s="21">
         <f>SUM(out_col0!A21:D40)</f>
-        <v>1180142</v>
+        <v>1269273</v>
       </c>
       <c r="Q6" s="21"/>
       <c r="R6" s="21"/>
@@ -755,16 +756,16 @@
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="4">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="B7" s="3">
-        <v>144</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4">
-        <v>84</v>
+        <v>169</v>
       </c>
       <c r="D7" s="3">
-        <v>224</v>
+        <v>175</v>
       </c>
       <c r="E7" s="23"/>
       <c r="O7" s="21">
@@ -772,7 +773,7 @@
       </c>
       <c r="P7" s="21">
         <f>SUM(out_col0!A41:D60)</f>
-        <v>1295681</v>
+        <v>1331389</v>
       </c>
       <c r="Q7" s="21"/>
       <c r="R7" s="21"/>
@@ -780,16 +781,16 @@
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="4">
-        <v>185</v>
+        <v>44</v>
       </c>
       <c r="B8" s="3">
-        <v>27</v>
+        <v>247</v>
       </c>
       <c r="C8" s="4">
-        <v>62</v>
+        <v>224</v>
       </c>
       <c r="D8" s="3">
-        <v>173</v>
+        <v>59</v>
       </c>
       <c r="E8" s="23"/>
       <c r="O8" s="21">
@@ -802,16 +803,16 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="4">
-        <v>20</v>
+        <v>245</v>
       </c>
       <c r="B9" s="3">
-        <v>39</v>
+        <v>205</v>
       </c>
       <c r="C9" s="4">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="D9" s="3">
-        <v>251</v>
+        <v>201</v>
       </c>
       <c r="E9" s="23"/>
       <c r="O9" s="21">
@@ -824,16 +825,16 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="6">
-        <v>194</v>
+        <v>142</v>
       </c>
       <c r="B10" s="5">
         <v>203</v>
       </c>
       <c r="C10" s="6">
-        <v>23</v>
+        <v>189</v>
       </c>
       <c r="D10" s="5">
-        <v>196</v>
+        <v>8</v>
       </c>
       <c r="E10" s="23"/>
       <c r="O10" s="21">
@@ -846,16 +847,16 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="1">
-        <v>130</v>
+        <v>198</v>
       </c>
       <c r="B11" s="2">
-        <v>124</v>
+        <v>60</v>
       </c>
       <c r="C11" s="1">
-        <v>229</v>
+        <v>251</v>
       </c>
       <c r="D11" s="2">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="E11" s="23"/>
       <c r="O11" s="21">
@@ -868,16 +869,16 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="3">
-        <v>221</v>
+        <v>174</v>
       </c>
       <c r="B12" s="4">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3">
-        <v>43</v>
+        <v>130</v>
       </c>
       <c r="D12" s="4">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E12" s="23"/>
       <c r="O12" s="21">
@@ -890,16 +891,16 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="3">
-        <v>209</v>
+        <v>67</v>
       </c>
       <c r="B13" s="4">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="C13" s="3">
-        <v>139</v>
+        <v>14</v>
       </c>
       <c r="D13" s="4">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="E13" s="23"/>
       <c r="O13" s="21">
@@ -912,121 +913,121 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="3">
-        <v>242</v>
+        <v>18</v>
       </c>
       <c r="B14" s="4">
-        <v>155</v>
+        <v>198</v>
       </c>
       <c r="C14" s="3">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="D14" s="4">
-        <v>247</v>
+        <v>17</v>
       </c>
       <c r="E14" s="23"/>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="5">
-        <v>241</v>
+        <v>203</v>
       </c>
       <c r="B15" s="6">
-        <v>56</v>
+        <v>242</v>
       </c>
       <c r="C15" s="5">
-        <v>5</v>
+        <v>121</v>
       </c>
       <c r="D15" s="6">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E15" s="23"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="2">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B16" s="1">
-        <v>145</v>
+        <v>84</v>
       </c>
       <c r="C16" s="2">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="D16" s="1">
-        <v>47</v>
+        <v>233</v>
       </c>
       <c r="E16" s="23"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="4">
-        <v>106</v>
+        <v>46</v>
       </c>
       <c r="B17" s="3">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C17" s="4">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="D17" s="3">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="E17" s="23"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="4">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="B18" s="3">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="C18" s="4">
-        <v>142</v>
+        <v>5</v>
       </c>
       <c r="D18" s="3">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="4">
-        <v>248</v>
+        <v>71</v>
       </c>
       <c r="B19" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C19" s="4">
-        <v>188</v>
+        <v>75</v>
       </c>
       <c r="D19" s="3">
-        <v>184</v>
+        <v>100</v>
       </c>
       <c r="E19" s="23"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="6">
-        <v>1</v>
+        <v>141</v>
       </c>
       <c r="B20" s="5">
-        <v>244</v>
+        <v>205</v>
       </c>
       <c r="C20" s="6">
-        <v>238</v>
+        <v>2</v>
       </c>
       <c r="D20" s="5">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="E20" s="23"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="B21" s="2">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="C21" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="2">
-        <v>104</v>
+        <v>200</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>1</v>
@@ -1034,301 +1035,301 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="B22" s="4">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="C22" s="3">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="D22" s="4">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E22" s="23"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3">
-        <v>50</v>
+        <v>207</v>
       </c>
       <c r="B23" s="4">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="C23" s="3">
-        <v>180</v>
+        <v>141</v>
       </c>
       <c r="D23" s="4">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="E23" s="23"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3">
-        <v>114</v>
+        <v>183</v>
       </c>
       <c r="B24" s="4">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="C24" s="3">
-        <v>9</v>
+        <v>192</v>
       </c>
       <c r="D24" s="4">
-        <v>210</v>
+        <v>23</v>
       </c>
       <c r="E24" s="23"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="5">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="B25" s="6">
-        <v>64</v>
+        <v>188</v>
       </c>
       <c r="C25" s="5">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D25" s="6">
-        <v>227</v>
+        <v>195</v>
       </c>
       <c r="E25" s="23"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2">
-        <v>128</v>
+        <v>180</v>
       </c>
       <c r="B26" s="1">
-        <v>231</v>
+        <v>23</v>
       </c>
       <c r="C26" s="2">
-        <v>208</v>
+        <v>134</v>
       </c>
       <c r="D26" s="1">
-        <v>214</v>
+        <v>157</v>
       </c>
       <c r="E26" s="23"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="4">
-        <v>0</v>
+        <v>179</v>
       </c>
       <c r="B27" s="3">
-        <v>56</v>
+        <v>253</v>
       </c>
       <c r="C27" s="4">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="D27" s="3">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="E27" s="23"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="4">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="B28" s="3">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="C28" s="4">
-        <v>222</v>
+        <v>160</v>
       </c>
       <c r="D28" s="3">
-        <v>112</v>
+        <v>10</v>
       </c>
       <c r="E28" s="23"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="4">
-        <v>236</v>
+        <v>30</v>
       </c>
       <c r="B29" s="3">
-        <v>178</v>
+        <v>113</v>
       </c>
       <c r="C29" s="4">
-        <v>198</v>
+        <v>243</v>
       </c>
       <c r="D29" s="3">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="E29" s="23"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="6">
-        <v>195</v>
+        <v>241</v>
       </c>
       <c r="B30" s="5">
-        <v>152</v>
+        <v>96</v>
       </c>
       <c r="C30" s="6">
-        <v>223</v>
+        <v>153</v>
       </c>
       <c r="D30" s="5">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="E30" s="23"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B31" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C31" s="1">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D31" s="2">
-        <v>57</v>
+        <v>215</v>
       </c>
       <c r="E31" s="23"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3">
-        <v>211</v>
+        <v>174</v>
       </c>
       <c r="B32" s="4">
-        <v>189</v>
+        <v>252</v>
       </c>
       <c r="C32" s="3">
-        <v>103</v>
+        <v>184</v>
       </c>
       <c r="D32" s="4">
-        <v>120</v>
+        <v>188</v>
       </c>
       <c r="E32" s="23"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3">
-        <v>252</v>
+        <v>125</v>
       </c>
       <c r="B33" s="4">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" s="3">
-        <v>87</v>
+        <v>205</v>
       </c>
       <c r="D33" s="4">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E33" s="23"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3">
-        <v>253</v>
+        <v>112</v>
       </c>
       <c r="B34" s="4">
-        <v>95</v>
+        <v>255</v>
       </c>
       <c r="C34" s="3">
-        <v>247</v>
+        <v>43</v>
       </c>
       <c r="D34" s="4">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="E34" s="23"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="5">
-        <v>14</v>
+        <v>216</v>
       </c>
       <c r="B35" s="6">
-        <v>212</v>
+        <v>13</v>
       </c>
       <c r="C35" s="5">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="D35" s="6">
-        <v>139</v>
+        <v>17</v>
       </c>
       <c r="E35" s="23"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="B36" s="1">
-        <v>44</v>
+        <v>153</v>
       </c>
       <c r="C36" s="2">
-        <v>216</v>
+        <v>139</v>
       </c>
       <c r="D36" s="1">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="E36" s="23"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="4">
-        <v>131</v>
+        <v>190</v>
       </c>
       <c r="B37" s="3">
-        <v>78</v>
+        <v>122</v>
       </c>
       <c r="C37" s="4">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="D37" s="3">
-        <v>204</v>
+        <v>55</v>
       </c>
       <c r="E37" s="23"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="4">
-        <v>255</v>
+        <v>48</v>
       </c>
       <c r="B38" s="3">
-        <v>126</v>
+        <v>41</v>
       </c>
       <c r="C38" s="4">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D38" s="3">
-        <v>221</v>
+        <v>81</v>
       </c>
       <c r="E38" s="23"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="4">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B39" s="3">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C39" s="4">
-        <v>161</v>
+        <v>208</v>
       </c>
       <c r="D39" s="3">
-        <v>39</v>
+        <v>216</v>
       </c>
       <c r="E39" s="23"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="6">
-        <v>28</v>
+        <v>129</v>
       </c>
       <c r="B40" s="5">
-        <v>205</v>
+        <v>98</v>
       </c>
       <c r="C40" s="6">
-        <v>34</v>
+        <v>143</v>
       </c>
       <c r="D40" s="5">
-        <v>110</v>
+        <v>185</v>
       </c>
       <c r="E40" s="23"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="7">
-        <v>177</v>
+        <v>220</v>
       </c>
       <c r="B41" s="8">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="C41" s="7">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="D41" s="8">
-        <v>207</v>
+        <v>33</v>
       </c>
       <c r="E41" s="23" t="s">
         <v>2</v>
@@ -1336,301 +1337,301 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="9">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="B42" s="10">
-        <v>139</v>
+        <v>65</v>
       </c>
       <c r="C42" s="9">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="D42" s="10">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E42" s="23"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="9">
-        <v>156</v>
+        <v>200</v>
       </c>
       <c r="B43" s="10">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="C43" s="9">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D43" s="10">
-        <v>161</v>
+        <v>209</v>
       </c>
       <c r="E43" s="23"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="9">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="B44" s="10">
-        <v>193</v>
+        <v>46</v>
       </c>
       <c r="C44" s="9">
-        <v>233</v>
+        <v>61</v>
       </c>
       <c r="D44" s="10">
-        <v>197</v>
+        <v>145</v>
       </c>
       <c r="E44" s="23"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="B45" s="12">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="C45" s="11">
-        <v>223</v>
+        <v>122</v>
       </c>
       <c r="D45" s="12">
-        <v>48</v>
+        <v>145</v>
       </c>
       <c r="E45" s="23"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="8">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B46" s="7">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="C46" s="8">
-        <v>99</v>
+        <v>210</v>
       </c>
       <c r="D46" s="7">
-        <v>15</v>
+        <v>135</v>
       </c>
       <c r="E46" s="23"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="10">
-        <v>37</v>
+        <v>107</v>
       </c>
       <c r="B47" s="9">
-        <v>182</v>
+        <v>137</v>
       </c>
       <c r="C47" s="10">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="D47" s="9">
-        <v>180</v>
+        <v>96</v>
       </c>
       <c r="E47" s="23"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="10">
-        <v>47</v>
+        <v>251</v>
       </c>
       <c r="B48" s="9">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="C48" s="10">
-        <v>128</v>
+        <v>25</v>
       </c>
       <c r="D48" s="9">
-        <v>55</v>
+        <v>118</v>
       </c>
       <c r="E48" s="23"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="10">
-        <v>159</v>
+        <v>43</v>
       </c>
       <c r="B49" s="9">
-        <v>20</v>
+        <v>178</v>
       </c>
       <c r="C49" s="10">
-        <v>114</v>
+        <v>229</v>
       </c>
       <c r="D49" s="9">
-        <v>205</v>
+        <v>17</v>
       </c>
       <c r="E49" s="23"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="12">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="B50" s="11">
         <v>4</v>
       </c>
       <c r="C50" s="12">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="D50" s="11">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="E50" s="23"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="7">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="B51" s="8">
-        <v>158</v>
+        <v>193</v>
       </c>
       <c r="C51" s="7">
-        <v>170</v>
+        <v>36</v>
       </c>
       <c r="D51" s="8">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="E51" s="23"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="9">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="B52" s="10">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="C52" s="9">
-        <v>146</v>
+        <v>81</v>
       </c>
       <c r="D52" s="10">
-        <v>10</v>
+        <v>202</v>
       </c>
       <c r="E52" s="23"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="9">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="B53" s="10">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C53" s="9">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="D53" s="10">
-        <v>251</v>
+        <v>216</v>
       </c>
       <c r="E53" s="23"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="9">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B54" s="10">
-        <v>88</v>
+        <v>244</v>
       </c>
       <c r="C54" s="9">
-        <v>116</v>
+        <v>208</v>
       </c>
       <c r="D54" s="10">
-        <v>107</v>
+        <v>46</v>
       </c>
       <c r="E54" s="23"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="11">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B55" s="12">
-        <v>195</v>
+        <v>163</v>
       </c>
       <c r="C55" s="11">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="D55" s="12">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="E55" s="23"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="8">
-        <v>183</v>
+        <v>204</v>
       </c>
       <c r="B56" s="7">
-        <v>216</v>
+        <v>18</v>
       </c>
       <c r="C56" s="8">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="D56" s="7">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="E56" s="23"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="10">
-        <v>152</v>
+        <v>234</v>
       </c>
       <c r="B57" s="9">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C57" s="10">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D57" s="9">
-        <v>181</v>
+        <v>255</v>
       </c>
       <c r="E57" s="23"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="10">
-        <v>247</v>
+        <v>124</v>
       </c>
       <c r="B58" s="9">
-        <v>188</v>
+        <v>158</v>
       </c>
       <c r="C58" s="10">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="D58" s="9">
-        <v>3</v>
+        <v>165</v>
       </c>
       <c r="E58" s="23"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="10">
-        <v>174</v>
+        <v>52</v>
       </c>
       <c r="B59" s="9">
-        <v>154</v>
+        <v>196</v>
       </c>
       <c r="C59" s="10">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D59" s="9">
-        <v>38</v>
+        <v>201</v>
       </c>
       <c r="E59" s="23"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="12">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B60" s="11">
-        <v>204</v>
+        <v>58</v>
       </c>
       <c r="C60" s="12">
-        <v>117</v>
+        <v>34</v>
       </c>
       <c r="D60" s="11">
-        <v>64</v>
+        <v>209</v>
       </c>
       <c r="E60" s="23"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="7">
-        <v>20</v>
+        <v>244</v>
       </c>
       <c r="B61" s="8">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="C61" s="7">
-        <v>188</v>
+        <v>16</v>
       </c>
       <c r="D61" s="8">
-        <v>207</v>
+        <v>164</v>
       </c>
       <c r="E61" s="23" t="s">
         <v>3</v>
@@ -1638,286 +1639,286 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="9">
-        <v>155</v>
+        <v>5</v>
       </c>
       <c r="B62" s="10">
-        <v>67</v>
+        <v>205</v>
       </c>
       <c r="C62" s="9">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="D62" s="10">
-        <v>112</v>
+        <v>180</v>
       </c>
       <c r="E62" s="23"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="9">
-        <v>155</v>
+        <v>239</v>
       </c>
       <c r="B63" s="10">
-        <v>61</v>
+        <v>228</v>
       </c>
       <c r="C63" s="9">
-        <v>94</v>
+        <v>149</v>
       </c>
       <c r="D63" s="10">
-        <v>182</v>
+        <v>105</v>
       </c>
       <c r="E63" s="23"/>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="9">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B64" s="10">
-        <v>215</v>
+        <v>71</v>
       </c>
       <c r="C64" s="9">
-        <v>184</v>
+        <v>12</v>
       </c>
       <c r="D64" s="10">
-        <v>103</v>
+        <v>166</v>
       </c>
       <c r="E64" s="23"/>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="11">
-        <v>169</v>
+        <v>251</v>
       </c>
       <c r="B65" s="12">
-        <v>204</v>
+        <v>84</v>
       </c>
       <c r="C65" s="11">
-        <v>119</v>
+        <v>75</v>
       </c>
       <c r="D65" s="12">
-        <v>245</v>
+        <v>136</v>
       </c>
       <c r="E65" s="23"/>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="8">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B66" s="7">
-        <v>183</v>
+        <v>243</v>
       </c>
       <c r="C66" s="8">
-        <v>217</v>
+        <v>171</v>
       </c>
       <c r="D66" s="7">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="E66" s="23"/>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="10">
-        <v>222</v>
+        <v>169</v>
       </c>
       <c r="B67" s="9">
-        <v>228</v>
+        <v>102</v>
       </c>
       <c r="C67" s="10">
-        <v>218</v>
+        <v>112</v>
       </c>
       <c r="D67" s="9">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E67" s="23"/>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="10">
-        <v>79</v>
+        <v>229</v>
       </c>
       <c r="B68" s="9">
-        <v>225</v>
+        <v>9</v>
       </c>
       <c r="C68" s="10">
-        <v>234</v>
+        <v>18</v>
       </c>
       <c r="D68" s="9">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="E68" s="23"/>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="10">
-        <v>65</v>
+        <v>248</v>
       </c>
       <c r="B69" s="9">
-        <v>246</v>
+        <v>152</v>
       </c>
       <c r="C69" s="10">
-        <v>93</v>
+        <v>191</v>
       </c>
       <c r="D69" s="9">
-        <v>192</v>
+        <v>25</v>
       </c>
       <c r="E69" s="23"/>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="12">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="B70" s="11">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="C70" s="12">
-        <v>121</v>
+        <v>62</v>
       </c>
       <c r="D70" s="11">
-        <v>166</v>
+        <v>236</v>
       </c>
       <c r="E70" s="23"/>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="7">
-        <v>111</v>
+        <v>188</v>
       </c>
       <c r="B71" s="8">
-        <v>213</v>
+        <v>60</v>
       </c>
       <c r="C71" s="7">
-        <v>189</v>
+        <v>228</v>
       </c>
       <c r="D71" s="8">
-        <v>95</v>
+        <v>172</v>
       </c>
       <c r="E71" s="23"/>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="9">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="B72" s="10">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="C72" s="9">
-        <v>28</v>
+        <v>247</v>
       </c>
       <c r="D72" s="10">
-        <v>113</v>
+        <v>226</v>
       </c>
       <c r="E72" s="23"/>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="9">
-        <v>155</v>
+        <v>19</v>
       </c>
       <c r="B73" s="10">
-        <v>70</v>
+        <v>240</v>
       </c>
       <c r="C73" s="9">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D73" s="10">
-        <v>203</v>
+        <v>49</v>
       </c>
       <c r="E73" s="23"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="9">
-        <v>53</v>
+        <v>142</v>
       </c>
       <c r="B74" s="10">
+        <v>126</v>
+      </c>
+      <c r="C74" s="9">
         <v>193</v>
       </c>
-      <c r="C74" s="9">
-        <v>89</v>
-      </c>
       <c r="D74" s="10">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="E74" s="23"/>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="11">
-        <v>169</v>
+        <v>33</v>
       </c>
       <c r="B75" s="12">
-        <v>229</v>
+        <v>4</v>
       </c>
       <c r="C75" s="11">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="D75" s="12">
-        <v>156</v>
+        <v>112</v>
       </c>
       <c r="E75" s="23"/>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="8">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B76" s="7">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C76" s="8">
-        <v>112</v>
+        <v>51</v>
       </c>
       <c r="D76" s="7">
-        <v>225</v>
+        <v>13</v>
       </c>
       <c r="E76" s="23"/>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="10">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="B77" s="9">
-        <v>52</v>
+        <v>217</v>
       </c>
       <c r="C77" s="10">
-        <v>250</v>
+        <v>61</v>
       </c>
       <c r="D77" s="9">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="E77" s="23"/>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="10">
-        <v>198</v>
+        <v>219</v>
       </c>
       <c r="B78" s="9">
-        <v>180</v>
+        <v>154</v>
       </c>
       <c r="C78" s="10">
-        <v>209</v>
+        <v>3</v>
       </c>
       <c r="D78" s="9">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="E78" s="23"/>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="10">
-        <v>212</v>
+        <v>18</v>
       </c>
       <c r="B79" s="9">
-        <v>171</v>
+        <v>139</v>
       </c>
       <c r="C79" s="10">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="D79" s="9">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="E79" s="23"/>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="12">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B80" s="11">
-        <v>246</v>
+        <v>30</v>
       </c>
       <c r="C80" s="12">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D80" s="11">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="E80" s="23"/>
     </row>
@@ -2607,248 +2608,258 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{642B7B6F-63FB-4815-8995-57121255FB68}">
-  <dimension ref="A1:G60"/>
+  <sheetPr codeName="Foglio2"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="10" max="10" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="A1" s="19">
         <f>Foglio1!A1*Foglio1!A81</f>
-        <v>13578</v>
+        <v>7440</v>
       </c>
       <c r="B1" s="19">
         <f>Foglio1!B1*Foglio1!B81</f>
-        <v>10836</v>
+        <v>20812</v>
       </c>
       <c r="C1" s="19">
         <f>Foglio1!C1*Foglio1!C81</f>
-        <v>35030</v>
+        <v>36890</v>
       </c>
       <c r="D1" s="19">
         <f>Foglio1!D1*Foglio1!D81</f>
-        <v>29082</v>
+        <v>28820</v>
       </c>
       <c r="E1" s="24"/>
       <c r="F1">
         <f>SUM(A1:D1)</f>
-        <v>88526</v>
-      </c>
-      <c r="G1">
+        <v>93962</v>
+      </c>
+      <c r="I1">
         <f>F1+F6+F11+F16</f>
-        <v>274777</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>313094</v>
+      </c>
+      <c r="J1" t="e">
+        <f>DEC2BIN(I1,32)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="19">
         <f>Foglio1!A2*Foglio1!A82</f>
-        <v>32670</v>
+        <v>13695</v>
       </c>
       <c r="B2" s="19">
         <f>Foglio1!B2*Foglio1!B82</f>
-        <v>11413</v>
+        <v>24521</v>
       </c>
       <c r="C2" s="19">
         <f>Foglio1!C2*Foglio1!C82</f>
-        <v>16092</v>
+        <v>37399</v>
       </c>
       <c r="D2" s="19">
         <f>Foglio1!D2*Foglio1!D82</f>
-        <v>16256</v>
+        <v>640</v>
       </c>
       <c r="E2" s="24"/>
       <c r="F2">
         <f t="shared" ref="F2:F20" si="0">SUM(A2:D2)</f>
-        <v>76431</v>
-      </c>
-      <c r="G2">
-        <f t="shared" ref="G2:G5" si="1">F2+F7+F12+F17</f>
-        <v>286534</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>76255</v>
+      </c>
+      <c r="I2">
+        <f>F2+F7+F12+F17</f>
+        <v>257372</v>
+      </c>
+      <c r="J2" t="e">
+        <f>DEC2BIN(I2,32)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="19">
         <f>Foglio1!A3*Foglio1!A83</f>
-        <v>42781</v>
+        <v>11950</v>
       </c>
       <c r="B3" s="19">
         <f>Foglio1!B3*Foglio1!B83</f>
-        <v>35964</v>
+        <v>10449</v>
       </c>
       <c r="C3" s="19">
         <f>Foglio1!C3*Foglio1!C83</f>
-        <v>5900</v>
+        <v>2675</v>
       </c>
       <c r="D3" s="19">
         <f>Foglio1!D3*Foglio1!D83</f>
-        <v>39120</v>
+        <v>39360</v>
       </c>
       <c r="E3" s="24"/>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>123765</v>
-      </c>
-      <c r="G3">
-        <f t="shared" si="1"/>
-        <v>255282</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>64434</v>
+      </c>
+      <c r="I3">
+        <f>F3+F8+F13+F18</f>
+        <v>141751</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="19">
         <f>Foglio1!A4*Foglio1!A84</f>
-        <v>23714</v>
+        <v>5344</v>
       </c>
       <c r="B4" s="19">
         <f>Foglio1!B4*Foglio1!B84</f>
-        <v>30940</v>
+        <v>14140</v>
       </c>
       <c r="C4" s="19">
         <f>Foglio1!C4*Foglio1!C84</f>
-        <v>4480</v>
+        <v>2548</v>
       </c>
       <c r="D4" s="19">
         <f>Foglio1!D4*Foglio1!D84</f>
-        <v>8004</v>
+        <v>1288</v>
       </c>
       <c r="E4" s="24"/>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>67138</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="1"/>
-        <v>265630</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>23320</v>
+      </c>
+      <c r="I4">
+        <f>F4+F9+F14+F19</f>
+        <v>174687</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="19">
         <f>Foglio1!A5*Foglio1!A85</f>
-        <v>11495</v>
+        <v>13365</v>
       </c>
       <c r="B5" s="19">
         <f>Foglio1!B5*Foglio1!B85</f>
-        <v>41584</v>
+        <v>17628</v>
       </c>
       <c r="C5" s="19">
         <f>Foglio1!C5*Foglio1!C85</f>
-        <v>9222</v>
+        <v>19836</v>
       </c>
       <c r="D5" s="19">
         <f>Foglio1!D5*Foglio1!D85</f>
-        <v>32</v>
+        <v>4192</v>
       </c>
       <c r="E5" s="24"/>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>62333</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="1"/>
-        <v>306170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>55021</v>
+      </c>
+      <c r="I5">
+        <f>F5+F10+F15+F20</f>
+        <v>270020</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="20">
         <f>Foglio1!A6*Foglio1!A90</f>
-        <v>41256</v>
+        <v>3888</v>
       </c>
       <c r="B6" s="20">
         <f>Foglio1!B6*Foglio1!B90</f>
-        <v>15200</v>
+        <v>48450</v>
       </c>
       <c r="C6" s="20">
         <f>Foglio1!C6*Foglio1!C90</f>
-        <v>16380</v>
+        <v>756</v>
       </c>
       <c r="D6" s="20">
         <f>Foglio1!D6*Foglio1!D90</f>
-        <v>5916</v>
+        <v>6596</v>
       </c>
       <c r="E6" s="24"/>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>78752</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>59690</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="20">
         <f>Foglio1!A7*Foglio1!A91</f>
-        <v>17976</v>
+        <v>14552</v>
       </c>
       <c r="B7" s="20">
         <f>Foglio1!B7*Foglio1!B91</f>
-        <v>20592</v>
+        <v>1716</v>
       </c>
       <c r="C7" s="20">
         <f>Foglio1!C7*Foglio1!C91</f>
-        <v>7140</v>
+        <v>14365</v>
       </c>
       <c r="D7" s="20">
         <f>Foglio1!D7*Foglio1!D91</f>
-        <v>48384</v>
+        <v>37800</v>
       </c>
       <c r="E7" s="24"/>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>94092</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>68433</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="20">
         <f>Foglio1!A8*Foglio1!A92</f>
-        <v>16280</v>
+        <v>3872</v>
       </c>
       <c r="B8" s="20">
         <f>Foglio1!B8*Foglio1!B92</f>
-        <v>378</v>
+        <v>3458</v>
       </c>
       <c r="C8" s="20">
         <f>Foglio1!C8*Foglio1!C92</f>
-        <v>4526</v>
+        <v>16352</v>
       </c>
       <c r="D8" s="20">
         <f>Foglio1!D8*Foglio1!D92</f>
-        <v>11418</v>
+        <v>3894</v>
       </c>
       <c r="E8" s="24"/>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>32602</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>27576</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="20">
         <f>Foglio1!A9*Foglio1!A93</f>
-        <v>880</v>
+        <v>10780</v>
       </c>
       <c r="B9" s="20">
         <f>Foglio1!B9*Foglio1!B93</f>
-        <v>4056</v>
+        <v>21320</v>
       </c>
       <c r="C9" s="20">
         <f>Foglio1!C9*Foglio1!C93</f>
-        <v>2940</v>
+        <v>17395</v>
       </c>
       <c r="D9" s="20">
         <f>Foglio1!D9*Foglio1!D93</f>
-        <v>14809</v>
+        <v>11859</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>22685</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>61354</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="20">
         <f>Foglio1!A10*Foglio1!A94</f>
-        <v>12610</v>
+        <v>9230</v>
       </c>
       <c r="B10" s="20">
         <f>Foglio1!B10*Foglio1!B94</f>
@@ -2856,959 +2867,959 @@
       </c>
       <c r="C10" s="20">
         <f>Foglio1!C10*Foglio1!C94</f>
-        <v>2783</v>
+        <v>22869</v>
       </c>
       <c r="D10" s="20">
         <f>Foglio1!D10*Foglio1!D94</f>
-        <v>43316</v>
+        <v>1768</v>
       </c>
       <c r="E10" s="24"/>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>67438</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>42596</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="19">
         <f>Foglio1!A11*Foglio1!A99</f>
-        <v>23920</v>
+        <v>36432</v>
       </c>
       <c r="B11" s="19">
         <f>Foglio1!B11*Foglio1!B99</f>
-        <v>23932</v>
+        <v>11580</v>
       </c>
       <c r="C11" s="19">
         <f>Foglio1!C11*Foglio1!C99</f>
-        <v>35953</v>
+        <v>39407</v>
       </c>
       <c r="D11" s="19">
         <f>Foglio1!D11*Foglio1!D99</f>
-        <v>9486</v>
+        <v>13464</v>
       </c>
       <c r="E11" s="24"/>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>93291</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>100883</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="19">
         <f>Foglio1!A12*Foglio1!A100</f>
-        <v>40001</v>
+        <v>31494</v>
       </c>
       <c r="B12" s="19">
         <f>Foglio1!B12*Foglio1!B100</f>
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="C12" s="19">
         <f>Foglio1!C12*Foglio1!C100</f>
-        <v>5977</v>
+        <v>18070</v>
       </c>
       <c r="D12" s="19">
         <f>Foglio1!D12*Foglio1!D100</f>
-        <v>1200</v>
+        <v>4800</v>
       </c>
       <c r="E12" s="24"/>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>47262</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>54395</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="19">
         <f>Foglio1!A13*Foglio1!A101</f>
-        <v>7315</v>
+        <v>2345</v>
       </c>
       <c r="B13" s="19">
         <f>Foglio1!B13*Foglio1!B101</f>
-        <v>12193</v>
+        <v>12905</v>
       </c>
       <c r="C13" s="19">
         <f>Foglio1!C13*Foglio1!C101</f>
-        <v>13066</v>
+        <v>1316</v>
       </c>
       <c r="D13" s="19">
         <f>Foglio1!D13*Foglio1!D101</f>
-        <v>19824</v>
+        <v>22176</v>
       </c>
       <c r="E13" s="24"/>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>52398</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>38742</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="19">
         <f>Foglio1!A14*Foglio1!A102</f>
-        <v>9438</v>
+        <v>702</v>
       </c>
       <c r="B14" s="19">
         <f>Foglio1!B14*Foglio1!B102</f>
-        <v>29915</v>
+        <v>38214</v>
       </c>
       <c r="C14" s="19">
         <f>Foglio1!C14*Foglio1!C102</f>
-        <v>26085</v>
+        <v>17390</v>
       </c>
       <c r="D14" s="19">
         <f>Foglio1!D14*Foglio1!D102</f>
-        <v>24206</v>
+        <v>1666</v>
       </c>
       <c r="E14" s="24"/>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>89644</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>57972</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="19">
         <f>Foglio1!A15*Foglio1!A103</f>
-        <v>54948</v>
+        <v>46284</v>
       </c>
       <c r="B15" s="19">
         <f>Foglio1!B15*Foglio1!B103</f>
-        <v>3304</v>
+        <v>14278</v>
       </c>
       <c r="C15" s="19">
         <f>Foglio1!C15*Foglio1!C103</f>
-        <v>760</v>
+        <v>18392</v>
       </c>
       <c r="D15" s="19">
         <f>Foglio1!D15*Foglio1!D103</f>
-        <v>30456</v>
+        <v>30832</v>
       </c>
       <c r="E15" s="24"/>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>89468</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>109786</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="20">
         <f>Foglio1!A16*Foglio1!A108</f>
-        <v>810</v>
+        <v>675</v>
       </c>
       <c r="B16" s="20">
         <f>Foglio1!B16*Foglio1!B108</f>
-        <v>435</v>
+        <v>252</v>
       </c>
       <c r="C16" s="20">
         <f>Foglio1!C16*Foglio1!C108</f>
-        <v>4550</v>
+        <v>15925</v>
       </c>
       <c r="D16" s="20">
         <f>Foglio1!D16*Foglio1!D108</f>
-        <v>8413</v>
+        <v>41707</v>
       </c>
       <c r="E16" s="24"/>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>14208</v>
+        <v>58559</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="20">
         <f>Foglio1!A17*Foglio1!A109</f>
-        <v>19080</v>
+        <v>8280</v>
       </c>
       <c r="B17" s="20">
         <f>Foglio1!B17*Foglio1!B109</f>
-        <v>33075</v>
+        <v>32200</v>
       </c>
       <c r="C17" s="20">
         <f>Foglio1!C17*Foglio1!C109</f>
-        <v>3796</v>
+        <v>5767</v>
       </c>
       <c r="D17" s="20">
         <f>Foglio1!D17*Foglio1!D109</f>
-        <v>12798</v>
+        <v>12042</v>
       </c>
       <c r="E17" s="24"/>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>68749</v>
+        <v>58289</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="20">
         <f>Foglio1!A18*Foglio1!A110</f>
-        <v>9476</v>
+        <v>8786</v>
       </c>
       <c r="B18" s="20">
         <f>Foglio1!B18*Foglio1!B110</f>
-        <v>16089</v>
+        <v>1038</v>
       </c>
       <c r="C18" s="20">
         <f>Foglio1!C18*Foglio1!C110</f>
-        <v>20022</v>
+        <v>705</v>
       </c>
       <c r="D18" s="20">
         <f>Foglio1!D18*Foglio1!D110</f>
-        <v>930</v>
+        <v>470</v>
       </c>
       <c r="E18" s="24"/>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>46517</v>
+        <v>10999</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="20">
         <f>Foglio1!A19*Foglio1!A111</f>
-        <v>61008</v>
+        <v>17466</v>
       </c>
       <c r="B19" s="20">
         <f>Foglio1!B19*Foglio1!B111</f>
-        <v>975</v>
+        <v>1950</v>
       </c>
       <c r="C19" s="20">
         <f>Foglio1!C19*Foglio1!C111</f>
-        <v>3572</v>
+        <v>1425</v>
       </c>
       <c r="D19" s="20">
         <f>Foglio1!D19*Foglio1!D111</f>
-        <v>20608</v>
+        <v>11200</v>
       </c>
       <c r="E19" s="24"/>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>86163</v>
+        <v>32041</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="20">
         <f>Foglio1!A20*Foglio1!A112</f>
-        <v>72</v>
+        <v>10152</v>
       </c>
       <c r="B20" s="20">
         <f>Foglio1!B20*Foglio1!B112</f>
-        <v>56608</v>
+        <v>47560</v>
       </c>
       <c r="C20" s="20">
         <f>Foglio1!C20*Foglio1!C112</f>
-        <v>20706</v>
+        <v>174</v>
       </c>
       <c r="D20" s="20">
         <f>Foglio1!D20*Foglio1!D112</f>
-        <v>9545</v>
+        <v>4731</v>
       </c>
       <c r="E20" s="24"/>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>86931</v>
+        <v>62617</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="19">
         <f>Foglio1!A21*Foglio1!A81</f>
-        <v>2697</v>
+        <v>16275</v>
       </c>
       <c r="B21" s="19">
         <f>Foglio1!B21*Foglio1!B81</f>
-        <v>19780</v>
+        <v>12040</v>
       </c>
       <c r="C21" s="19">
         <f>Foglio1!C21*Foglio1!C81</f>
-        <v>6510</v>
+        <v>6355</v>
       </c>
       <c r="D21" s="19">
         <f>Foglio1!D21*Foglio1!D81</f>
-        <v>13624</v>
+        <v>26200</v>
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="22">
         <f>SUM(A21:D21)</f>
-        <v>42611</v>
+        <v>60870</v>
       </c>
       <c r="G21" s="22">
         <f>F21+F26+F31+F36</f>
-        <v>213636</v>
+        <v>215605</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="19">
         <f>Foglio1!A22*Foglio1!A82</f>
-        <v>31515</v>
+        <v>24090</v>
       </c>
       <c r="B22" s="19">
         <f>Foglio1!B22*Foglio1!B82</f>
-        <v>7797</v>
+        <v>12204</v>
       </c>
       <c r="C22" s="19">
         <f>Foglio1!C22*Foglio1!C82</f>
-        <v>19817</v>
+        <v>0</v>
       </c>
       <c r="D22" s="19">
         <f>Foglio1!D22*Foglio1!D82</f>
-        <v>3648</v>
+        <v>64</v>
       </c>
       <c r="E22" s="26"/>
       <c r="F22">
-        <f t="shared" ref="F22:F40" si="2">SUM(A22:D22)</f>
-        <v>62777</v>
+        <f t="shared" ref="F22:F40" si="1">SUM(A22:D22)</f>
+        <v>36358</v>
       </c>
       <c r="G22">
-        <f t="shared" ref="G22:G25" si="3">F22+F27+F32+F37</f>
-        <v>223927</v>
+        <f t="shared" ref="G22:G25" si="2">F22+F27+F32+F37</f>
+        <v>269856</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="19">
         <f>Foglio1!A23*Foglio1!A83</f>
-        <v>11950</v>
+        <v>49473</v>
       </c>
       <c r="B23" s="19">
         <f>Foglio1!B23*Foglio1!B83</f>
-        <v>4374</v>
+        <v>23571</v>
       </c>
       <c r="C23" s="19">
         <f>Foglio1!C23*Foglio1!C83</f>
-        <v>4500</v>
+        <v>3525</v>
       </c>
       <c r="D23" s="19">
         <f>Foglio1!D23*Foglio1!D83</f>
-        <v>54240</v>
+        <v>56160</v>
       </c>
       <c r="E23" s="26"/>
       <c r="F23">
+        <f t="shared" si="1"/>
+        <v>132729</v>
+      </c>
+      <c r="G23">
         <f t="shared" si="2"/>
-        <v>75064</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="3"/>
-        <v>194670</v>
+        <v>219938</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="19">
         <f>Foglio1!A24*Foglio1!A84</f>
-        <v>19038</v>
+        <v>30561</v>
       </c>
       <c r="B24" s="19">
         <f>Foglio1!B24*Foglio1!B84</f>
-        <v>7840</v>
+        <v>15400</v>
       </c>
       <c r="C24" s="19">
         <f>Foglio1!C24*Foglio1!C84</f>
-        <v>252</v>
+        <v>5376</v>
       </c>
       <c r="D24" s="19">
         <f>Foglio1!D24*Foglio1!D84</f>
-        <v>19320</v>
+        <v>2116</v>
       </c>
       <c r="E24" s="26"/>
       <c r="F24">
+        <f t="shared" si="1"/>
+        <v>53453</v>
+      </c>
+      <c r="G24">
         <f t="shared" si="2"/>
-        <v>46450</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="3"/>
-        <v>310120</v>
+        <v>307046</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="19">
         <f>Foglio1!A25*Foglio1!A85</f>
-        <v>10230</v>
+        <v>8745</v>
       </c>
       <c r="B25" s="19">
         <f>Foglio1!B25*Foglio1!B85</f>
-        <v>14464</v>
+        <v>42488</v>
       </c>
       <c r="C25" s="19">
         <f>Foglio1!C25*Foglio1!C85</f>
-        <v>9048</v>
+        <v>7656</v>
       </c>
       <c r="D25" s="19">
         <f>Foglio1!D25*Foglio1!D85</f>
-        <v>7264</v>
+        <v>6240</v>
       </c>
       <c r="E25" s="26"/>
       <c r="F25">
+        <f t="shared" si="1"/>
+        <v>65129</v>
+      </c>
+      <c r="G25">
         <f t="shared" si="2"/>
-        <v>41006</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="3"/>
-        <v>237789</v>
+        <v>256828</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="20">
         <f>Foglio1!A26*Foglio1!A90</f>
-        <v>27648</v>
+        <v>38880</v>
       </c>
       <c r="B26" s="20">
         <f>Foglio1!B26*Foglio1!B90</f>
-        <v>43890</v>
+        <v>4370</v>
       </c>
       <c r="C26" s="20">
         <f>Foglio1!C26*Foglio1!C90</f>
-        <v>17472</v>
+        <v>11256</v>
       </c>
       <c r="D26" s="20">
         <f>Foglio1!D26*Foglio1!D90</f>
-        <v>7276</v>
+        <v>5338</v>
       </c>
       <c r="E26" s="26"/>
       <c r="F26">
-        <f t="shared" si="2"/>
-        <v>96286</v>
+        <f t="shared" si="1"/>
+        <v>59844</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="20">
         <f>Foglio1!A27*Foglio1!A91</f>
-        <v>0</v>
+        <v>19153</v>
       </c>
       <c r="B27" s="20">
         <f>Foglio1!B27*Foglio1!B91</f>
-        <v>8008</v>
+        <v>36179</v>
       </c>
       <c r="C27" s="20">
         <f>Foglio1!C27*Foglio1!C91</f>
-        <v>9265</v>
+        <v>10880</v>
       </c>
       <c r="D27" s="20">
         <f>Foglio1!D27*Foglio1!D91</f>
-        <v>38448</v>
+        <v>42552</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27">
-        <f t="shared" si="2"/>
-        <v>55721</v>
+        <f t="shared" si="1"/>
+        <v>108764</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="20">
         <f>Foglio1!A28*Foglio1!A92</f>
-        <v>3784</v>
+        <v>0</v>
       </c>
       <c r="B28" s="20">
         <f>Foglio1!B28*Foglio1!B92</f>
-        <v>84</v>
+        <v>742</v>
       </c>
       <c r="C28" s="20">
         <f>Foglio1!C28*Foglio1!C92</f>
-        <v>16206</v>
+        <v>11680</v>
       </c>
       <c r="D28" s="20">
         <f>Foglio1!D28*Foglio1!D92</f>
-        <v>7392</v>
+        <v>660</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28">
-        <f t="shared" si="2"/>
-        <v>27466</v>
+        <f t="shared" si="1"/>
+        <v>13082</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="20">
         <f>Foglio1!A29*Foglio1!A93</f>
-        <v>10384</v>
+        <v>1320</v>
       </c>
       <c r="B29" s="20">
         <f>Foglio1!B29*Foglio1!B93</f>
-        <v>18512</v>
+        <v>11752</v>
       </c>
       <c r="C29" s="20">
         <f>Foglio1!C29*Foglio1!C93</f>
-        <v>48510</v>
+        <v>59535</v>
       </c>
       <c r="D29" s="20">
         <f>Foglio1!D29*Foglio1!D93</f>
-        <v>12803</v>
+        <v>13098</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29">
-        <f t="shared" si="2"/>
-        <v>90209</v>
+        <f t="shared" si="1"/>
+        <v>85705</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="20">
         <f>Foglio1!A30*Foglio1!A94</f>
-        <v>12675</v>
+        <v>15665</v>
       </c>
       <c r="B30" s="20">
         <f>Foglio1!B30*Foglio1!B94</f>
-        <v>6536</v>
+        <v>4128</v>
       </c>
       <c r="C30" s="20">
         <f>Foglio1!C30*Foglio1!C94</f>
-        <v>26983</v>
+        <v>18513</v>
       </c>
       <c r="D30" s="20">
         <f>Foglio1!D30*Foglio1!D94</f>
-        <v>32045</v>
+        <v>35802</v>
       </c>
       <c r="E30" s="26"/>
       <c r="F30">
-        <f t="shared" si="2"/>
-        <v>78239</v>
+        <f t="shared" si="1"/>
+        <v>74108</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19">
         <f>Foglio1!A31*Foglio1!A99</f>
-        <v>8832</v>
+        <v>9016</v>
       </c>
       <c r="B31" s="19">
         <f>Foglio1!B31*Foglio1!B99</f>
-        <v>772</v>
+        <v>579</v>
       </c>
       <c r="C31" s="19">
         <f>Foglio1!C31*Foglio1!C99</f>
-        <v>2512</v>
+        <v>471</v>
       </c>
       <c r="D31" s="19">
         <f>Foglio1!D31*Foglio1!D99</f>
-        <v>8721</v>
+        <v>32895</v>
       </c>
       <c r="E31" s="26"/>
       <c r="F31">
-        <f t="shared" si="2"/>
-        <v>20837</v>
+        <f t="shared" si="1"/>
+        <v>42961</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="19">
         <f>Foglio1!A32*Foglio1!A100</f>
-        <v>38191</v>
+        <v>31494</v>
       </c>
       <c r="B32" s="19">
         <f>Foglio1!B32*Foglio1!B100</f>
-        <v>189</v>
+        <v>252</v>
       </c>
       <c r="C32" s="19">
         <f>Foglio1!C32*Foglio1!C100</f>
-        <v>14317</v>
+        <v>25576</v>
       </c>
       <c r="D32" s="19">
         <f>Foglio1!D32*Foglio1!D100</f>
-        <v>2880</v>
+        <v>4512</v>
       </c>
       <c r="E32" s="26"/>
       <c r="F32">
-        <f t="shared" si="2"/>
-        <v>55577</v>
+        <f t="shared" si="1"/>
+        <v>61834</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19">
         <f>Foglio1!A33*Foglio1!A101</f>
-        <v>8820</v>
+        <v>4375</v>
       </c>
       <c r="B33" s="19">
         <f>Foglio1!B33*Foglio1!B101</f>
-        <v>3560</v>
+        <v>3471</v>
       </c>
       <c r="C33" s="19">
         <f>Foglio1!C33*Foglio1!C101</f>
-        <v>8178</v>
+        <v>19270</v>
       </c>
       <c r="D33" s="19">
         <f>Foglio1!D33*Foglio1!D101</f>
-        <v>3696</v>
+        <v>5880</v>
       </c>
       <c r="E33" s="26"/>
       <c r="F33">
-        <f t="shared" si="2"/>
-        <v>24254</v>
+        <f t="shared" si="1"/>
+        <v>32996</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19">
         <f>Foglio1!A34*Foglio1!A102</f>
-        <v>9867</v>
+        <v>4368</v>
       </c>
       <c r="B34" s="19">
         <f>Foglio1!B34*Foglio1!B102</f>
-        <v>18335</v>
+        <v>49215</v>
       </c>
       <c r="C34" s="19">
         <f>Foglio1!C34*Foglio1!C102</f>
-        <v>58045</v>
+        <v>10105</v>
       </c>
       <c r="D34" s="19">
         <f>Foglio1!D34*Foglio1!D102</f>
-        <v>6860</v>
+        <v>3528</v>
       </c>
       <c r="E34" s="26"/>
       <c r="F34">
-        <f t="shared" si="2"/>
-        <v>93107</v>
+        <f t="shared" si="1"/>
+        <v>67216</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19">
         <f>Foglio1!A35*Foglio1!A103</f>
-        <v>3192</v>
+        <v>49248</v>
       </c>
       <c r="B35" s="19">
         <f>Foglio1!B35*Foglio1!B103</f>
-        <v>12508</v>
+        <v>767</v>
       </c>
       <c r="C35" s="19">
         <f>Foglio1!C35*Foglio1!C103</f>
-        <v>15048</v>
+        <v>4560</v>
       </c>
       <c r="D35" s="19">
         <f>Foglio1!D35*Foglio1!D103</f>
-        <v>26132</v>
+        <v>3196</v>
       </c>
       <c r="E35" s="26"/>
       <c r="F35">
-        <f t="shared" si="2"/>
-        <v>56880</v>
+        <f t="shared" si="1"/>
+        <v>57771</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="20">
         <f>Foglio1!A36*Foglio1!A108</f>
-        <v>576</v>
+        <v>117</v>
       </c>
       <c r="B36" s="20">
         <f>Foglio1!B36*Foglio1!B108</f>
-        <v>132</v>
+        <v>459</v>
       </c>
       <c r="C36" s="20">
         <f>Foglio1!C36*Foglio1!C108</f>
-        <v>37800</v>
+        <v>24325</v>
       </c>
       <c r="D36" s="20">
         <f>Foglio1!D36*Foglio1!D108</f>
-        <v>15394</v>
+        <v>27029</v>
       </c>
       <c r="E36" s="26"/>
       <c r="F36">
-        <f t="shared" si="2"/>
-        <v>53902</v>
+        <f t="shared" si="1"/>
+        <v>51930</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="20">
         <f>Foglio1!A37*Foglio1!A109</f>
-        <v>23580</v>
+        <v>34200</v>
       </c>
       <c r="B37" s="20">
         <f>Foglio1!B37*Foglio1!B109</f>
-        <v>13650</v>
+        <v>21350</v>
       </c>
       <c r="C37" s="20">
         <f>Foglio1!C37*Foglio1!C109</f>
-        <v>1606</v>
+        <v>4380</v>
       </c>
       <c r="D37" s="20">
         <f>Foglio1!D37*Foglio1!D109</f>
-        <v>11016</v>
+        <v>2970</v>
       </c>
       <c r="E37" s="26"/>
       <c r="F37">
-        <f t="shared" si="2"/>
-        <v>49852</v>
+        <f t="shared" si="1"/>
+        <v>62900</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="20">
         <f>Foglio1!A38*Foglio1!A110</f>
-        <v>11730</v>
+        <v>2208</v>
       </c>
       <c r="B38" s="20">
         <f>Foglio1!B38*Foglio1!B110</f>
-        <v>21798</v>
+        <v>7093</v>
       </c>
       <c r="C38" s="20">
         <f>Foglio1!C38*Foglio1!C110</f>
-        <v>32148</v>
+        <v>31020</v>
       </c>
       <c r="D38" s="20">
         <f>Foglio1!D38*Foglio1!D110</f>
-        <v>2210</v>
+        <v>810</v>
       </c>
       <c r="E38" s="26"/>
       <c r="F38">
-        <f t="shared" si="2"/>
-        <v>67886</v>
+        <f t="shared" si="1"/>
+        <v>41131</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="20">
         <f>Foglio1!A39*Foglio1!A111</f>
-        <v>58302</v>
+        <v>57318</v>
       </c>
       <c r="B39" s="20">
         <f>Foglio1!B39*Foglio1!B111</f>
-        <v>14625</v>
+        <v>15210</v>
       </c>
       <c r="C39" s="20">
         <f>Foglio1!C39*Foglio1!C111</f>
-        <v>3059</v>
+        <v>3952</v>
       </c>
       <c r="D39" s="20">
         <f>Foglio1!D39*Foglio1!D111</f>
-        <v>4368</v>
+        <v>24192</v>
       </c>
       <c r="E39" s="26"/>
       <c r="F39">
-        <f t="shared" si="2"/>
-        <v>80354</v>
+        <f t="shared" si="1"/>
+        <v>100672</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="20">
         <f>Foglio1!A40*Foglio1!A112</f>
-        <v>2016</v>
+        <v>9288</v>
       </c>
       <c r="B40" s="20">
         <f>Foglio1!B40*Foglio1!B112</f>
-        <v>47560</v>
+        <v>22736</v>
       </c>
       <c r="C40" s="20">
         <f>Foglio1!C40*Foglio1!C112</f>
-        <v>2958</v>
+        <v>12441</v>
       </c>
       <c r="D40" s="20">
         <f>Foglio1!D40*Foglio1!D112</f>
-        <v>9130</v>
+        <v>15355</v>
       </c>
       <c r="E40" s="26"/>
       <c r="F40">
-        <f t="shared" si="2"/>
-        <v>61664</v>
+        <f t="shared" si="1"/>
+        <v>59820</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="19">
         <f>Foglio1!A41*Foglio1!A81</f>
-        <v>16461</v>
+        <v>20460</v>
       </c>
       <c r="B41" s="19">
         <f>Foglio1!B41*Foglio1!B81</f>
-        <v>17372</v>
+        <v>5332</v>
       </c>
       <c r="C41" s="19">
         <f>Foglio1!C41*Foglio1!C81</f>
-        <v>35495</v>
+        <v>37355</v>
       </c>
       <c r="D41" s="19">
         <f>Foglio1!D41*Foglio1!D81</f>
-        <v>27117</v>
+        <v>4323</v>
       </c>
       <c r="E41" s="27"/>
       <c r="F41" s="22">
         <f>SUM(A41:D41)</f>
-        <v>96445</v>
+        <v>67470</v>
       </c>
       <c r="G41" s="22">
         <f>F41+F46+F51+F56</f>
-        <v>298990</v>
+        <v>266408</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19">
         <f>Foglio1!A42*Foglio1!A82</f>
-        <v>34485</v>
+        <v>38115</v>
       </c>
       <c r="B42" s="19">
         <f>Foglio1!B42*Foglio1!B82</f>
-        <v>15707</v>
+        <v>7345</v>
       </c>
       <c r="C42" s="19">
         <f>Foglio1!C42*Foglio1!C82</f>
-        <v>6705</v>
+        <v>13112</v>
       </c>
       <c r="D42" s="19">
         <f>Foglio1!D42*Foglio1!D82</f>
-        <v>1280</v>
+        <v>768</v>
       </c>
       <c r="E42" s="27"/>
       <c r="F42">
-        <f t="shared" ref="F42:F60" si="4">SUM(A42:D42)</f>
-        <v>58177</v>
+        <f t="shared" ref="F42:F60" si="3">SUM(A42:D42)</f>
+        <v>59340</v>
       </c>
       <c r="G42">
-        <f t="shared" ref="G42:G45" si="5">F42+F47+F52+F57</f>
-        <v>249639</v>
+        <f t="shared" ref="G42:G45" si="4">F42+F47+F52+F57</f>
+        <v>256273</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="19">
         <f>Foglio1!A43*Foglio1!A83</f>
-        <v>37284</v>
+        <v>47800</v>
       </c>
       <c r="B43" s="19">
         <f>Foglio1!B43*Foglio1!B83</f>
-        <v>5103</v>
+        <v>23328</v>
       </c>
       <c r="C43" s="19">
         <f>Foglio1!C43*Foglio1!C83</f>
-        <v>850</v>
+        <v>1300</v>
       </c>
       <c r="D43" s="19">
         <f>Foglio1!D43*Foglio1!D83</f>
-        <v>38640</v>
+        <v>50160</v>
       </c>
       <c r="E43" s="27"/>
       <c r="F43">
+        <f t="shared" si="3"/>
+        <v>122588</v>
+      </c>
+      <c r="G43">
         <f t="shared" si="4"/>
-        <v>81877</v>
-      </c>
-      <c r="G43">
-        <f t="shared" si="5"/>
-        <v>208051</v>
+        <v>254531</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="19">
         <f>Foglio1!A44*Foglio1!A84</f>
-        <v>28390</v>
+        <v>33567</v>
       </c>
       <c r="B44" s="19">
         <f>Foglio1!B44*Foglio1!B84</f>
-        <v>27020</v>
+        <v>6440</v>
       </c>
       <c r="C44" s="19">
         <f>Foglio1!C44*Foglio1!C84</f>
-        <v>6524</v>
+        <v>1708</v>
       </c>
       <c r="D44" s="19">
         <f>Foglio1!D44*Foglio1!D84</f>
-        <v>18124</v>
+        <v>13340</v>
       </c>
       <c r="E44" s="27"/>
       <c r="F44">
+        <f t="shared" si="3"/>
+        <v>55055</v>
+      </c>
+      <c r="G44">
         <f t="shared" si="4"/>
-        <v>80058</v>
-      </c>
-      <c r="G44">
-        <f t="shared" si="5"/>
-        <v>264532</v>
+        <v>312754</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="19">
         <f>Foglio1!A45*Foglio1!A85</f>
-        <v>5005</v>
+        <v>6765</v>
       </c>
       <c r="B45" s="19">
         <f>Foglio1!B45*Foglio1!B85</f>
-        <v>18080</v>
+        <v>7910</v>
       </c>
       <c r="C45" s="19">
         <f>Foglio1!C45*Foglio1!C85</f>
-        <v>38802</v>
+        <v>21228</v>
       </c>
       <c r="D45" s="19">
         <f>Foglio1!D45*Foglio1!D85</f>
-        <v>1536</v>
+        <v>4640</v>
       </c>
       <c r="E45" s="27"/>
       <c r="F45">
+        <f t="shared" si="3"/>
+        <v>40543</v>
+      </c>
+      <c r="G45">
         <f t="shared" si="4"/>
-        <v>63423</v>
-      </c>
-      <c r="G45">
-        <f t="shared" si="5"/>
-        <v>274469</v>
+        <v>241423</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="20">
         <f>Foglio1!A90*Foglio1!A46</f>
-        <v>33264</v>
+        <v>31320</v>
       </c>
       <c r="B46" s="20">
         <f>Foglio1!B90*Foglio1!B46</f>
-        <v>16910</v>
+        <v>11970</v>
       </c>
       <c r="C46" s="20">
         <f>Foglio1!C90*Foglio1!C46</f>
-        <v>8316</v>
+        <v>17640</v>
       </c>
       <c r="D46" s="20">
         <f>Foglio1!D90*Foglio1!D46</f>
-        <v>510</v>
+        <v>4590</v>
       </c>
       <c r="E46" s="27"/>
       <c r="F46">
-        <f t="shared" si="4"/>
-        <v>59000</v>
+        <f t="shared" si="3"/>
+        <v>65520</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="20">
         <f>Foglio1!A91*Foglio1!A47</f>
-        <v>3959</v>
+        <v>11449</v>
       </c>
       <c r="B47" s="20">
         <f>Foglio1!B91*Foglio1!B47</f>
-        <v>26026</v>
+        <v>19591</v>
       </c>
       <c r="C47" s="20">
         <f>Foglio1!C91*Foglio1!C47</f>
-        <v>6120</v>
+        <v>8075</v>
       </c>
       <c r="D47" s="20">
         <f>Foglio1!D91*Foglio1!D47</f>
-        <v>38880</v>
+        <v>20736</v>
       </c>
       <c r="E47" s="27"/>
       <c r="F47">
-        <f t="shared" si="4"/>
-        <v>74985</v>
+        <f t="shared" si="3"/>
+        <v>59851</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="20">
         <f>Foglio1!A92*Foglio1!A48</f>
-        <v>4136</v>
+        <v>22088</v>
       </c>
       <c r="B48" s="20">
         <f>Foglio1!B92*Foglio1!B48</f>
-        <v>2310</v>
+        <v>2534</v>
       </c>
       <c r="C48" s="20">
         <f>Foglio1!C92*Foglio1!C48</f>
-        <v>9344</v>
+        <v>1825</v>
       </c>
       <c r="D48" s="20">
         <f>Foglio1!D92*Foglio1!D48</f>
-        <v>3630</v>
+        <v>7788</v>
       </c>
       <c r="E48" s="27"/>
       <c r="F48">
-        <f t="shared" si="4"/>
-        <v>19420</v>
+        <f t="shared" si="3"/>
+        <v>34235</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="20">
         <f>Foglio1!A93*Foglio1!A49</f>
-        <v>6996</v>
+        <v>1892</v>
       </c>
       <c r="B49" s="20">
         <f>Foglio1!B93*Foglio1!B49</f>
-        <v>2080</v>
+        <v>18512</v>
       </c>
       <c r="C49" s="20">
         <f>Foglio1!C93*Foglio1!C49</f>
-        <v>27930</v>
+        <v>56105</v>
       </c>
       <c r="D49" s="20">
         <f>Foglio1!D93*Foglio1!D49</f>
-        <v>12095</v>
+        <v>1003</v>
       </c>
       <c r="E49" s="27"/>
       <c r="F49">
-        <f t="shared" si="4"/>
-        <v>49101</v>
+        <f t="shared" si="3"/>
+        <v>77512</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="20">
         <f>Foglio1!A94*Foglio1!A50</f>
-        <v>7800</v>
+        <v>845</v>
       </c>
       <c r="B50" s="20">
         <f>Foglio1!B94*Foglio1!B50</f>
@@ -3816,246 +3827,246 @@
       </c>
       <c r="C50" s="20">
         <f>Foglio1!C94*Foglio1!C50</f>
-        <v>26499</v>
+        <v>27467</v>
       </c>
       <c r="D50" s="20">
         <f>Foglio1!D94*Foglio1!D50</f>
-        <v>44863</v>
+        <v>48178</v>
       </c>
       <c r="E50" s="27"/>
       <c r="F50">
-        <f t="shared" si="4"/>
-        <v>79334</v>
+        <f t="shared" si="3"/>
+        <v>76662</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="19">
         <f>Foglio1!A51*Foglio1!A99</f>
-        <v>18400</v>
+        <v>23184</v>
       </c>
       <c r="B51" s="19">
         <f>Foglio1!B51*Foglio1!B99</f>
-        <v>30494</v>
+        <v>37249</v>
       </c>
       <c r="C51" s="19">
         <f>Foglio1!C51*Foglio1!C99</f>
-        <v>26690</v>
+        <v>5652</v>
       </c>
       <c r="D51" s="19">
         <f>Foglio1!D51*Foglio1!D99</f>
-        <v>32895</v>
+        <v>34884</v>
       </c>
       <c r="E51" s="27"/>
       <c r="F51">
-        <f t="shared" si="4"/>
-        <v>108479</v>
+        <f t="shared" si="3"/>
+        <v>100969</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="19">
         <f>Foglio1!A52*Foglio1!A100</f>
-        <v>25340</v>
+        <v>32580</v>
       </c>
       <c r="B52" s="19">
         <f>Foglio1!B52*Foglio1!B100</f>
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="C52" s="19">
         <f>Foglio1!C52*Foglio1!C100</f>
-        <v>20294</v>
+        <v>11259</v>
       </c>
       <c r="D52" s="19">
         <f>Foglio1!D52*Foglio1!D100</f>
-        <v>240</v>
+        <v>4848</v>
       </c>
       <c r="E52" s="27"/>
       <c r="F52">
-        <f t="shared" si="4"/>
-        <v>45889</v>
+        <f t="shared" si="3"/>
+        <v>48759</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="19">
         <f>Foglio1!A53*Foglio1!A101</f>
-        <v>3220</v>
+        <v>1330</v>
       </c>
       <c r="B53" s="19">
         <f>Foglio1!B53*Foglio1!B101</f>
-        <v>3115</v>
+        <v>4628</v>
       </c>
       <c r="C53" s="19">
         <f>Foglio1!C53*Foglio1!C101</f>
-        <v>6580</v>
+        <v>2726</v>
       </c>
       <c r="D53" s="19">
         <f>Foglio1!D53*Foglio1!D101</f>
-        <v>42168</v>
+        <v>36288</v>
       </c>
       <c r="E53" s="27"/>
       <c r="F53">
-        <f t="shared" si="4"/>
-        <v>55083</v>
+        <f t="shared" si="3"/>
+        <v>44972</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="19">
         <f>Foglio1!A54*Foglio1!A102</f>
-        <v>741</v>
+        <v>3276</v>
       </c>
       <c r="B54" s="19">
         <f>Foglio1!B54*Foglio1!B102</f>
-        <v>16984</v>
+        <v>47092</v>
       </c>
       <c r="C54" s="19">
         <f>Foglio1!C54*Foglio1!C102</f>
-        <v>27260</v>
+        <v>48880</v>
       </c>
       <c r="D54" s="19">
         <f>Foglio1!D54*Foglio1!D102</f>
-        <v>10486</v>
+        <v>4508</v>
       </c>
       <c r="E54" s="27"/>
       <c r="F54">
-        <f t="shared" si="4"/>
-        <v>55471</v>
+        <f t="shared" si="3"/>
+        <v>103756</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="19">
         <f>Foglio1!A55*Foglio1!A103</f>
-        <v>31236</v>
+        <v>29868</v>
       </c>
       <c r="B55" s="19">
         <f>Foglio1!B55*Foglio1!B103</f>
-        <v>11505</v>
+        <v>9617</v>
       </c>
       <c r="C55" s="19">
         <f>Foglio1!C55*Foglio1!C103</f>
-        <v>21128</v>
+        <v>26296</v>
       </c>
       <c r="D55" s="19">
         <f>Foglio1!D55*Foglio1!D103</f>
-        <v>3008</v>
+        <v>22372</v>
       </c>
       <c r="E55" s="27"/>
       <c r="F55">
-        <f t="shared" si="4"/>
-        <v>66877</v>
+        <f t="shared" si="3"/>
+        <v>88153</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="20">
         <f>Foglio1!A56*Foglio1!A108</f>
-        <v>1647</v>
+        <v>1836</v>
       </c>
       <c r="B56" s="20">
         <f>Foglio1!B56*Foglio1!B108</f>
-        <v>648</v>
+        <v>54</v>
       </c>
       <c r="C56" s="20">
         <f>Foglio1!C56*Foglio1!C108</f>
-        <v>15050</v>
+        <v>17850</v>
       </c>
       <c r="D56" s="20">
         <f>Foglio1!D56*Foglio1!D108</f>
-        <v>17721</v>
+        <v>12709</v>
       </c>
       <c r="E56" s="27"/>
       <c r="F56">
-        <f t="shared" si="4"/>
-        <v>35066</v>
+        <f t="shared" si="3"/>
+        <v>32449</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="20">
         <f>Foglio1!A57*Foglio1!A109</f>
-        <v>27360</v>
+        <v>42120</v>
       </c>
       <c r="B57" s="20">
         <f>Foglio1!B57*Foglio1!B109</f>
-        <v>20825</v>
+        <v>19950</v>
       </c>
       <c r="C57" s="20">
         <f>Foglio1!C57*Foglio1!C109</f>
-        <v>12629</v>
+        <v>12483</v>
       </c>
       <c r="D57" s="20">
         <f>Foglio1!D57*Foglio1!D109</f>
-        <v>9774</v>
+        <v>13770</v>
       </c>
       <c r="E57" s="27"/>
       <c r="F57">
-        <f t="shared" si="4"/>
-        <v>70588</v>
+        <f t="shared" si="3"/>
+        <v>88323</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="20">
         <f>Foglio1!A58*Foglio1!A110</f>
-        <v>11362</v>
+        <v>5704</v>
       </c>
       <c r="B58" s="20">
         <f>Foglio1!B58*Foglio1!B110</f>
-        <v>32524</v>
+        <v>27334</v>
       </c>
       <c r="C58" s="20">
         <f>Foglio1!C58*Foglio1!C110</f>
-        <v>7755</v>
+        <v>18048</v>
       </c>
       <c r="D58" s="20">
         <f>Foglio1!D58*Foglio1!D110</f>
-        <v>30</v>
+        <v>1650</v>
       </c>
       <c r="E58" s="27"/>
       <c r="F58">
-        <f t="shared" si="4"/>
-        <v>51671</v>
+        <f t="shared" si="3"/>
+        <v>52736</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="20">
         <f>Foglio1!A59*Foglio1!A111</f>
-        <v>42804</v>
+        <v>12792</v>
       </c>
       <c r="B59" s="20">
         <f>Foglio1!B59*Foglio1!B111</f>
-        <v>30030</v>
+        <v>38220</v>
       </c>
       <c r="C59" s="20">
         <f>Foglio1!C59*Foglio1!C111</f>
-        <v>2812</v>
+        <v>2907</v>
       </c>
       <c r="D59" s="20">
         <f>Foglio1!D59*Foglio1!D111</f>
-        <v>4256</v>
+        <v>22512</v>
       </c>
       <c r="E59" s="27"/>
       <c r="F59">
-        <f t="shared" si="4"/>
-        <v>79902</v>
+        <f t="shared" si="3"/>
+        <v>76431</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="20">
         <f>Foglio1!A60*Foglio1!A112</f>
-        <v>2016</v>
+        <v>2304</v>
       </c>
       <c r="B60" s="20">
         <f>Foglio1!B60*Foglio1!B112</f>
-        <v>47328</v>
+        <v>13456</v>
       </c>
       <c r="C60" s="20">
         <f>Foglio1!C60*Foglio1!C112</f>
-        <v>10179</v>
+        <v>2958</v>
       </c>
       <c r="D60" s="20">
         <f>Foglio1!D60*Foglio1!D112</f>
-        <v>5312</v>
+        <v>17347</v>
       </c>
       <c r="E60" s="27"/>
       <c r="F60">
-        <f t="shared" si="4"/>
-        <v>64835</v>
+        <f t="shared" si="3"/>
+        <v>36065</v>
       </c>
     </row>
   </sheetData>
@@ -4070,6 +4081,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9381655-1C82-4EE2-8B9E-D0B27E1AE275}">
+  <sheetPr codeName="Foglio3"/>
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4081,266 +4093,266 @@
     <row r="1" spans="1:11">
       <c r="A1" s="19">
         <f>Foglio1!A1*Foglio1!A82</f>
-        <v>24090</v>
+        <v>13200</v>
       </c>
       <c r="B1" s="19">
         <f>Foglio1!B1*Foglio1!B82</f>
-        <v>7119</v>
+        <v>13673</v>
       </c>
       <c r="C1" s="19">
         <f>Foglio1!C1*Foglio1!C82</f>
-        <v>33674</v>
+        <v>35462</v>
       </c>
       <c r="D1" s="19">
         <f>Foglio1!D1*Foglio1!D82</f>
-        <v>14208</v>
+        <v>14080</v>
       </c>
       <c r="E1" s="26"/>
       <c r="F1">
         <f>SUM(A1:D1)</f>
-        <v>79091</v>
+        <v>76415</v>
       </c>
       <c r="G1">
         <f>F1+F6+F11+F16</f>
-        <v>268111</v>
+        <v>277799</v>
       </c>
       <c r="H1">
         <f>SUM(A1:A5)</f>
-        <v>136076</v>
+        <v>74494</v>
       </c>
       <c r="I1">
         <f t="shared" ref="I1:K1" si="0">SUM(B1:B5)</f>
-        <v>146304</v>
+        <v>113892</v>
       </c>
       <c r="J1">
         <f t="shared" si="0"/>
-        <v>82853</v>
+        <v>86445</v>
       </c>
       <c r="K1">
         <f t="shared" si="0"/>
-        <v>93142</v>
+        <v>57430</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="19">
         <f>Foglio1!A2*Foglio1!A83</f>
-        <v>47322</v>
+        <v>19837</v>
       </c>
       <c r="B2" s="19">
         <f>Foglio1!B2*Foglio1!B83</f>
-        <v>24543</v>
+        <v>52731</v>
       </c>
       <c r="C2" s="19">
         <f>Foglio1!C2*Foglio1!C83</f>
-        <v>2700</v>
+        <v>6275</v>
       </c>
       <c r="D2" s="19">
         <f>Foglio1!D2*Foglio1!D83</f>
-        <v>60960</v>
+        <v>2400</v>
       </c>
       <c r="E2" s="26"/>
       <c r="F2">
         <f t="shared" ref="F2:F20" si="1">SUM(A2:D2)</f>
-        <v>135525</v>
+        <v>81243</v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G5" si="2">F2+F7+F12+F17</f>
-        <v>248169</v>
+        <v>219252</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="19">
         <f>Foglio1!A3*Foglio1!A84</f>
-        <v>29893</v>
+        <v>8350</v>
       </c>
       <c r="B3" s="19">
         <f>Foglio1!B3*Foglio1!B84</f>
-        <v>20720</v>
+        <v>6020</v>
       </c>
       <c r="C3" s="19">
         <f>Foglio1!C3*Foglio1!C84</f>
-        <v>6608</v>
+        <v>2996</v>
       </c>
       <c r="D3" s="19">
         <f>Foglio1!D3*Foglio1!D84</f>
-        <v>14996</v>
+        <v>15088</v>
       </c>
       <c r="E3" s="26"/>
       <c r="F3">
         <f t="shared" si="1"/>
-        <v>72217</v>
+        <v>32454</v>
       </c>
       <c r="G3">
         <f t="shared" si="2"/>
-        <v>269308</v>
+        <v>218778</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="19">
         <f>Foglio1!A4*Foglio1!A85</f>
-        <v>7810</v>
+        <v>1760</v>
       </c>
       <c r="B4" s="19">
         <f>Foglio1!B4*Foglio1!B85</f>
-        <v>49946</v>
+        <v>22826</v>
       </c>
       <c r="C4" s="19">
         <f>Foglio1!C4*Foglio1!C85</f>
-        <v>27840</v>
+        <v>15834</v>
       </c>
       <c r="D4" s="19">
         <f>Foglio1!D4*Foglio1!D85</f>
-        <v>2784</v>
+        <v>448</v>
       </c>
       <c r="E4" s="26"/>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>88380</v>
+        <v>40868</v>
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
-        <v>326553</v>
+        <v>171107</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="19">
         <f>Foglio1!A5*Foglio1!A86</f>
-        <v>26961</v>
+        <v>31347</v>
       </c>
       <c r="B5" s="19">
         <f>Foglio1!B5*Foglio1!B86</f>
-        <v>43976</v>
+        <v>18642</v>
       </c>
       <c r="C5" s="19">
         <f>Foglio1!C5*Foglio1!C86</f>
-        <v>12031</v>
+        <v>25878</v>
       </c>
       <c r="D5" s="19">
         <f>Foglio1!D5*Foglio1!D86</f>
-        <v>194</v>
+        <v>25414</v>
       </c>
       <c r="E5" s="26"/>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>83162</v>
+        <v>101281</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>293754</v>
+        <v>315518</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="20">
         <f>Foglio1!A6*Foglio1!A91</f>
-        <v>20437</v>
+        <v>1926</v>
       </c>
       <c r="B6" s="20">
         <f>Foglio1!B6*Foglio1!B91</f>
-        <v>11440</v>
+        <v>36465</v>
       </c>
       <c r="C6" s="20">
         <f>Foglio1!C6*Foglio1!C91</f>
-        <v>16575</v>
+        <v>765</v>
       </c>
       <c r="D6" s="20">
         <f>Foglio1!D6*Foglio1!D91</f>
-        <v>37584</v>
+        <v>41904</v>
       </c>
       <c r="E6" s="26"/>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>86036</v>
+        <v>81060</v>
       </c>
       <c r="H6">
         <f>SUM(A6:A10)</f>
-        <v>66195</v>
+        <v>47517</v>
       </c>
       <c r="I6">
         <f t="shared" ref="I6" si="3">SUM(B6:B10)</f>
-        <v>38647</v>
+        <v>91842</v>
       </c>
       <c r="J6">
         <f t="shared" ref="J6" si="4">SUM(C6:C10)</f>
-        <v>42362</v>
+        <v>101332</v>
       </c>
       <c r="K6">
         <f t="shared" ref="K6" si="5">SUM(D6:D10)</f>
-        <v>154502</v>
+        <v>102844</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="20">
         <f>Foglio1!A7*Foglio1!A92</f>
-        <v>14784</v>
+        <v>11968</v>
       </c>
       <c r="B7" s="20">
         <f>Foglio1!B7*Foglio1!B92</f>
-        <v>2016</v>
+        <v>168</v>
       </c>
       <c r="C7" s="20">
         <f>Foglio1!C7*Foglio1!C92</f>
-        <v>6132</v>
+        <v>12337</v>
       </c>
       <c r="D7" s="20">
         <f>Foglio1!D7*Foglio1!D92</f>
-        <v>14784</v>
+        <v>11550</v>
       </c>
       <c r="E7" s="26"/>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>37716</v>
+        <v>36023</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="20">
         <f>Foglio1!A8*Foglio1!A93</f>
-        <v>8140</v>
+        <v>1936</v>
       </c>
       <c r="B8" s="20">
         <f>Foglio1!B8*Foglio1!B93</f>
-        <v>2808</v>
+        <v>25688</v>
       </c>
       <c r="C8" s="20">
         <f>Foglio1!C8*Foglio1!C93</f>
-        <v>15190</v>
+        <v>54880</v>
       </c>
       <c r="D8" s="20">
         <f>Foglio1!D8*Foglio1!D93</f>
-        <v>10207</v>
+        <v>3481</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>36345</v>
+        <v>85985</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="20">
         <f>Foglio1!A9*Foglio1!A94</f>
-        <v>1300</v>
+        <v>15925</v>
       </c>
       <c r="B9" s="20">
         <f>Foglio1!B9*Foglio1!B94</f>
-        <v>1677</v>
+        <v>8815</v>
       </c>
       <c r="C9" s="20">
         <f>Foglio1!C9*Foglio1!C94</f>
-        <v>1452</v>
+        <v>8591</v>
       </c>
       <c r="D9" s="20">
         <f>Foglio1!D9*Foglio1!D94</f>
-        <v>55471</v>
+        <v>44421</v>
       </c>
       <c r="E9" s="26"/>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>59900</v>
+        <v>77752</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="20">
         <f>Foglio1!A10*Foglio1!A95</f>
-        <v>21534</v>
+        <v>15762</v>
       </c>
       <c r="B10" s="20">
         <f>Foglio1!B10*Foglio1!B95</f>
@@ -4348,278 +4360,278 @@
       </c>
       <c r="C10" s="20">
         <f>Foglio1!C10*Foglio1!C95</f>
-        <v>3013</v>
+        <v>24759</v>
       </c>
       <c r="D10" s="20">
         <f>Foglio1!D10*Foglio1!D95</f>
-        <v>36456</v>
+        <v>1488</v>
       </c>
       <c r="E10" s="26"/>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>81709</v>
+        <v>62715</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="19">
         <f>Foglio1!A11*Foglio1!A100</f>
-        <v>23530</v>
+        <v>35838</v>
       </c>
       <c r="B11" s="19">
         <f>Foglio1!B11*Foglio1!B100</f>
-        <v>124</v>
+        <v>60</v>
       </c>
       <c r="C11" s="19">
         <f>Foglio1!C11*Foglio1!C100</f>
-        <v>31831</v>
+        <v>34889</v>
       </c>
       <c r="D11" s="19">
         <f>Foglio1!D11*Foglio1!D100</f>
-        <v>1488</v>
+        <v>2112</v>
       </c>
       <c r="E11" s="26"/>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>56973</v>
+        <v>72899</v>
       </c>
       <c r="H11">
         <f>SUM(A11:A15)</f>
-        <v>126404</v>
+        <v>75441</v>
       </c>
       <c r="I11">
         <f t="shared" ref="I11" si="6">SUM(B11:B15)</f>
-        <v>50690</v>
+        <v>74914</v>
       </c>
       <c r="J11">
         <f t="shared" ref="J11" si="7">SUM(C11:C15)</f>
-        <v>86095</v>
+        <v>78224</v>
       </c>
       <c r="K11">
         <f t="shared" ref="K11" si="8">SUM(D11:D15)</f>
-        <v>68698</v>
+        <v>52664</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="19">
         <f>Foglio1!A12*Foglio1!A101</f>
-        <v>7735</v>
+        <v>6090</v>
       </c>
       <c r="B12" s="19">
         <f>Foglio1!B12*Foglio1!B101</f>
-        <v>7476</v>
+        <v>2759</v>
       </c>
       <c r="C12" s="19">
         <f>Foglio1!C12*Foglio1!C101</f>
-        <v>4042</v>
+        <v>12220</v>
       </c>
       <c r="D12" s="19">
         <f>Foglio1!D12*Foglio1!D101</f>
-        <v>8400</v>
+        <v>33600</v>
       </c>
       <c r="E12" s="26"/>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>27653</v>
+        <v>54669</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="19">
         <f>Foglio1!A13*Foglio1!A102</f>
-        <v>8151</v>
+        <v>2613</v>
       </c>
       <c r="B13" s="19">
         <f>Foglio1!B13*Foglio1!B102</f>
-        <v>26441</v>
+        <v>27985</v>
       </c>
       <c r="C13" s="19">
         <f>Foglio1!C13*Foglio1!C102</f>
-        <v>32665</v>
+        <v>3290</v>
       </c>
       <c r="D13" s="19">
         <f>Foglio1!D13*Foglio1!D102</f>
-        <v>11564</v>
+        <v>12936</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>78821</v>
+        <v>46824</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="19">
         <f>Foglio1!A14*Foglio1!A103</f>
-        <v>55176</v>
+        <v>4104</v>
       </c>
       <c r="B14" s="19">
         <f>Foglio1!B14*Foglio1!B103</f>
-        <v>9145</v>
+        <v>11682</v>
       </c>
       <c r="C14" s="19">
         <f>Foglio1!C14*Foglio1!C103</f>
-        <v>16872</v>
+        <v>11248</v>
       </c>
       <c r="D14" s="19">
         <f>Foglio1!D14*Foglio1!D103</f>
-        <v>46436</v>
+        <v>3196</v>
       </c>
       <c r="E14" s="26"/>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>127629</v>
+        <v>30230</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="19">
         <f>Foglio1!A15*Foglio1!A104</f>
-        <v>31812</v>
+        <v>26796</v>
       </c>
       <c r="B15" s="19">
         <f>Foglio1!B15*Foglio1!B104</f>
-        <v>7504</v>
+        <v>32428</v>
       </c>
       <c r="C15" s="19">
         <f>Foglio1!C15*Foglio1!C104</f>
-        <v>685</v>
+        <v>16577</v>
       </c>
       <c r="D15" s="19">
         <f>Foglio1!D15*Foglio1!D104</f>
-        <v>810</v>
+        <v>820</v>
       </c>
       <c r="E15" s="26"/>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>40811</v>
+        <v>76621</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="20">
         <f>Foglio1!A16*Foglio1!A109</f>
-        <v>16200</v>
+        <v>13500</v>
       </c>
       <c r="B16" s="20">
         <f>Foglio1!B16*Foglio1!B109</f>
-        <v>25375</v>
+        <v>14700</v>
       </c>
       <c r="C16" s="20">
         <f>Foglio1!C16*Foglio1!C109</f>
-        <v>1898</v>
+        <v>6643</v>
       </c>
       <c r="D16" s="20">
         <f>Foglio1!D16*Foglio1!D109</f>
-        <v>2538</v>
+        <v>12582</v>
       </c>
       <c r="E16" s="26"/>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>46011</v>
+        <v>47425</v>
       </c>
       <c r="H16">
         <f>SUM(A16:A20)</f>
-        <v>89721</v>
+        <v>83647</v>
       </c>
       <c r="I16">
         <f t="shared" ref="I16" si="9">SUM(B16:B20)</f>
-        <v>132755</v>
+        <v>96557</v>
       </c>
       <c r="J16">
         <f t="shared" ref="J16" si="10">SUM(C16:C20)</f>
-        <v>35900</v>
+        <v>24466</v>
       </c>
       <c r="K16">
         <f t="shared" ref="K16" si="11">SUM(D16:D20)</f>
-        <v>55551</v>
+        <v>40745</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="20">
         <f>Foglio1!A17*Foglio1!A110</f>
-        <v>4876</v>
+        <v>2116</v>
       </c>
       <c r="B17" s="20">
         <f>Foglio1!B17*Foglio1!B110</f>
-        <v>32697</v>
+        <v>31832</v>
       </c>
       <c r="C17" s="20">
         <f>Foglio1!C17*Foglio1!C110</f>
-        <v>7332</v>
+        <v>11139</v>
       </c>
       <c r="D17" s="20">
         <f>Foglio1!D17*Foglio1!D110</f>
-        <v>2370</v>
+        <v>2230</v>
       </c>
       <c r="E17" s="26"/>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>47275</v>
+        <v>47317</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="20">
         <f>Foglio1!A18*Foglio1!A111</f>
-        <v>50676</v>
+        <v>46986</v>
       </c>
       <c r="B18" s="20">
         <f>Foglio1!B18*Foglio1!B111</f>
-        <v>18135</v>
+        <v>1170</v>
       </c>
       <c r="C18" s="20">
         <f>Foglio1!C18*Foglio1!C111</f>
-        <v>2698</v>
+        <v>95</v>
       </c>
       <c r="D18" s="20">
         <f>Foglio1!D18*Foglio1!D111</f>
-        <v>10416</v>
+        <v>5264</v>
       </c>
       <c r="E18" s="26"/>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>81925</v>
+        <v>53515</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="20">
         <f>Foglio1!A19*Foglio1!A112</f>
-        <v>17856</v>
+        <v>5112</v>
       </c>
       <c r="B19" s="20">
         <f>Foglio1!B19*Foglio1!B112</f>
-        <v>1160</v>
+        <v>2320</v>
       </c>
       <c r="C19" s="20">
         <f>Foglio1!C19*Foglio1!C112</f>
-        <v>16356</v>
+        <v>6525</v>
       </c>
       <c r="D19" s="20">
         <f>Foglio1!D19*Foglio1!D112</f>
-        <v>15272</v>
+        <v>8300</v>
       </c>
       <c r="E19" s="26"/>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>50644</v>
+        <v>22257</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="20">
         <f>Foglio1!A20*Foglio1!A113</f>
-        <v>113</v>
+        <v>15933</v>
       </c>
       <c r="B20" s="20">
         <f>Foglio1!B20*Foglio1!B113</f>
-        <v>55388</v>
+        <v>46535</v>
       </c>
       <c r="C20" s="20">
         <f>Foglio1!C20*Foglio1!C113</f>
-        <v>7616</v>
+        <v>64</v>
       </c>
       <c r="D20" s="20">
         <f>Foglio1!D20*Foglio1!D113</f>
-        <v>24955</v>
+        <v>12369</v>
       </c>
       <c r="E20" s="26"/>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>88072</v>
+        <v>74901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testato fino al rimo replace sample
</commit_message>
<xml_diff>
--- a/test_conv1d/test_conv1d/mem.xlsx
+++ b/test_conv1d/test_conv1d/mem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Titania\Desktop\ms\lab3\test_conv1d\test_conv1d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80859B24-E829-40A6-BC36-C2AC17E626FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0698451C-B8B2-48C1-A065-753F33332214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="12960" windowHeight="9690" xr2:uid="{0D9A6957-12B8-4496-A02D-3AD1E515C0C0}"/>
+    <workbookView xWindow="0" yWindow="1230" windowWidth="14085" windowHeight="9690" xr2:uid="{0D9A6957-12B8-4496-A02D-3AD1E515C0C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -619,16 +619,16 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1">
-        <v>80</v>
+        <v>146</v>
       </c>
       <c r="B1" s="2">
-        <v>121</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="D1" s="2">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E1" s="23" t="s">
         <v>0</v>
@@ -636,31 +636,31 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="3">
-        <v>83</v>
+        <v>198</v>
       </c>
       <c r="B2" s="4">
-        <v>217</v>
+        <v>101</v>
       </c>
       <c r="C2" s="3">
-        <v>251</v>
+        <v>108</v>
       </c>
       <c r="D2" s="4">
-        <v>10</v>
+        <v>254</v>
       </c>
       <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="3">
-        <v>50</v>
+        <v>179</v>
       </c>
       <c r="B3" s="4">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="C3" s="3">
-        <v>107</v>
+        <v>236</v>
       </c>
       <c r="D3" s="4">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E3" s="23"/>
       <c r="O3" s="21"/>
@@ -673,16 +673,16 @@
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="3">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="B4" s="4">
-        <v>101</v>
+        <v>221</v>
       </c>
       <c r="C4" s="3">
-        <v>91</v>
+        <v>160</v>
       </c>
       <c r="D4" s="4">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="E4" s="23"/>
       <c r="O4" s="21" t="s">
@@ -703,16 +703,16 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="5">
-        <v>243</v>
+        <v>209</v>
       </c>
       <c r="B5" s="6">
-        <v>78</v>
+        <v>184</v>
       </c>
       <c r="C5" s="5">
-        <v>114</v>
+        <v>53</v>
       </c>
       <c r="D5" s="6">
-        <v>131</v>
+        <v>1</v>
       </c>
       <c r="E5" s="23"/>
       <c r="O5" s="21">
@@ -720,27 +720,27 @@
       </c>
       <c r="P5" s="21">
         <f>SUM(out_col0!A1:D20)</f>
-        <v>1156924</v>
+        <v>1276566</v>
       </c>
       <c r="Q5">
         <f>SUM(out_col1!A1:D20)</f>
-        <v>1202454</v>
+        <v>1216911</v>
       </c>
       <c r="R5" s="21"/>
       <c r="S5" s="21"/>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="2">
-        <v>18</v>
+        <v>191</v>
       </c>
       <c r="B6" s="1">
-        <v>255</v>
+        <v>80</v>
       </c>
       <c r="C6" s="2">
-        <v>9</v>
+        <v>195</v>
       </c>
       <c r="D6" s="1">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="E6" s="23"/>
       <c r="O6" s="21">
@@ -748,7 +748,7 @@
       </c>
       <c r="P6" s="21">
         <f>SUM(out_col0!A21:D40)</f>
-        <v>1269273</v>
+        <v>1174096</v>
       </c>
       <c r="Q6" s="21"/>
       <c r="R6" s="21"/>
@@ -756,16 +756,16 @@
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="4">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="B7" s="3">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="C7" s="4">
-        <v>169</v>
+        <v>84</v>
       </c>
       <c r="D7" s="3">
-        <v>175</v>
+        <v>224</v>
       </c>
       <c r="E7" s="23"/>
       <c r="O7" s="21">
@@ -773,7 +773,7 @@
       </c>
       <c r="P7" s="21">
         <f>SUM(out_col0!A41:D60)</f>
-        <v>1331389</v>
+        <v>1198256</v>
       </c>
       <c r="Q7" s="21"/>
       <c r="R7" s="21"/>
@@ -781,16 +781,16 @@
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="4">
-        <v>44</v>
+        <v>185</v>
       </c>
       <c r="B8" s="3">
-        <v>247</v>
+        <v>27</v>
       </c>
       <c r="C8" s="4">
-        <v>224</v>
+        <v>62</v>
       </c>
       <c r="D8" s="3">
-        <v>59</v>
+        <v>173</v>
       </c>
       <c r="E8" s="23"/>
       <c r="O8" s="21">
@@ -803,16 +803,16 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="4">
-        <v>245</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3">
-        <v>205</v>
+        <v>39</v>
       </c>
       <c r="C9" s="4">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="D9" s="3">
-        <v>201</v>
+        <v>251</v>
       </c>
       <c r="E9" s="23"/>
       <c r="O9" s="21">
@@ -825,16 +825,16 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="6">
-        <v>142</v>
+        <v>194</v>
       </c>
       <c r="B10" s="5">
         <v>203</v>
       </c>
       <c r="C10" s="6">
-        <v>189</v>
+        <v>23</v>
       </c>
       <c r="D10" s="5">
-        <v>8</v>
+        <v>196</v>
       </c>
       <c r="E10" s="23"/>
       <c r="O10" s="21">
@@ -847,16 +847,16 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="1">
-        <v>198</v>
+        <v>130</v>
       </c>
       <c r="B11" s="2">
-        <v>60</v>
+        <v>124</v>
       </c>
       <c r="C11" s="1">
-        <v>251</v>
+        <v>229</v>
       </c>
       <c r="D11" s="2">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="E11" s="23"/>
       <c r="O11" s="21">
@@ -869,16 +869,16 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="3">
-        <v>174</v>
+        <v>221</v>
       </c>
       <c r="B12" s="4">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="C12" s="3">
-        <v>130</v>
+        <v>43</v>
       </c>
       <c r="D12" s="4">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E12" s="23"/>
       <c r="O12" s="21">
@@ -891,16 +891,16 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="3">
-        <v>67</v>
+        <v>209</v>
       </c>
       <c r="B13" s="4">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C13" s="3">
-        <v>14</v>
+        <v>139</v>
       </c>
       <c r="D13" s="4">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="E13" s="23"/>
       <c r="O13" s="21">
@@ -913,121 +913,121 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="3">
-        <v>18</v>
+        <v>242</v>
       </c>
       <c r="B14" s="4">
-        <v>198</v>
+        <v>155</v>
       </c>
       <c r="C14" s="3">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="D14" s="4">
-        <v>17</v>
+        <v>247</v>
       </c>
       <c r="E14" s="23"/>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="5">
-        <v>203</v>
+        <v>241</v>
       </c>
       <c r="B15" s="6">
-        <v>242</v>
+        <v>56</v>
       </c>
       <c r="C15" s="5">
-        <v>121</v>
+        <v>5</v>
       </c>
       <c r="D15" s="6">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E15" s="23"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="2">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="B16" s="1">
-        <v>84</v>
+        <v>145</v>
       </c>
       <c r="C16" s="2">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="D16" s="1">
-        <v>233</v>
+        <v>47</v>
       </c>
       <c r="E16" s="23"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="4">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="B17" s="3">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C17" s="4">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="D17" s="3">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="E17" s="23"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="4">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="B18" s="3">
-        <v>6</v>
+        <v>93</v>
       </c>
       <c r="C18" s="4">
-        <v>5</v>
+        <v>142</v>
       </c>
       <c r="D18" s="3">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="4">
-        <v>71</v>
+        <v>248</v>
       </c>
       <c r="B19" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C19" s="4">
-        <v>75</v>
+        <v>188</v>
       </c>
       <c r="D19" s="3">
-        <v>100</v>
+        <v>184</v>
       </c>
       <c r="E19" s="23"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="6">
-        <v>141</v>
+        <v>1</v>
       </c>
       <c r="B20" s="5">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="C20" s="6">
-        <v>2</v>
+        <v>238</v>
       </c>
       <c r="D20" s="5">
-        <v>57</v>
+        <v>115</v>
       </c>
       <c r="E20" s="23"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1">
-        <v>175</v>
+        <v>29</v>
       </c>
       <c r="B21" s="2">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="C21" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D21" s="2">
-        <v>200</v>
+        <v>104</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>1</v>
@@ -1035,301 +1035,301 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3">
-        <v>146</v>
+        <v>191</v>
       </c>
       <c r="B22" s="4">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="C22" s="3">
-        <v>0</v>
+        <v>133</v>
       </c>
       <c r="D22" s="4">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E22" s="23"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3">
-        <v>207</v>
+        <v>50</v>
       </c>
       <c r="B23" s="4">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="C23" s="3">
-        <v>141</v>
+        <v>180</v>
       </c>
       <c r="D23" s="4">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E23" s="23"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3">
-        <v>183</v>
+        <v>114</v>
       </c>
       <c r="B24" s="4">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="C24" s="3">
-        <v>192</v>
+        <v>9</v>
       </c>
       <c r="D24" s="4">
-        <v>23</v>
+        <v>210</v>
       </c>
       <c r="E24" s="23"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="5">
-        <v>159</v>
+        <v>186</v>
       </c>
       <c r="B25" s="6">
-        <v>188</v>
+        <v>64</v>
       </c>
       <c r="C25" s="5">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D25" s="6">
-        <v>195</v>
+        <v>227</v>
       </c>
       <c r="E25" s="23"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2">
-        <v>180</v>
+        <v>128</v>
       </c>
       <c r="B26" s="1">
-        <v>23</v>
+        <v>231</v>
       </c>
       <c r="C26" s="2">
-        <v>134</v>
+        <v>208</v>
       </c>
       <c r="D26" s="1">
-        <v>157</v>
+        <v>214</v>
       </c>
       <c r="E26" s="23"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="4">
-        <v>179</v>
+        <v>0</v>
       </c>
       <c r="B27" s="3">
-        <v>253</v>
+        <v>56</v>
       </c>
       <c r="C27" s="4">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="D27" s="3">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="E27" s="23"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="4">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="B28" s="3">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="C28" s="4">
-        <v>160</v>
+        <v>222</v>
       </c>
       <c r="D28" s="3">
-        <v>10</v>
+        <v>112</v>
       </c>
       <c r="E28" s="23"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="4">
-        <v>30</v>
+        <v>236</v>
       </c>
       <c r="B29" s="3">
-        <v>113</v>
+        <v>178</v>
       </c>
       <c r="C29" s="4">
-        <v>243</v>
+        <v>198</v>
       </c>
       <c r="D29" s="3">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E29" s="23"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="6">
-        <v>241</v>
+        <v>195</v>
       </c>
       <c r="B30" s="5">
-        <v>96</v>
+        <v>152</v>
       </c>
       <c r="C30" s="6">
-        <v>153</v>
+        <v>223</v>
       </c>
       <c r="D30" s="5">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="E30" s="23"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C31" s="1">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D31" s="2">
-        <v>215</v>
+        <v>57</v>
       </c>
       <c r="E31" s="23"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3">
-        <v>174</v>
+        <v>211</v>
       </c>
       <c r="B32" s="4">
-        <v>252</v>
+        <v>189</v>
       </c>
       <c r="C32" s="3">
-        <v>184</v>
+        <v>103</v>
       </c>
       <c r="D32" s="4">
-        <v>188</v>
+        <v>120</v>
       </c>
       <c r="E32" s="23"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3">
-        <v>125</v>
+        <v>252</v>
       </c>
       <c r="B33" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C33" s="3">
-        <v>205</v>
+        <v>87</v>
       </c>
       <c r="D33" s="4">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E33" s="23"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3">
-        <v>112</v>
+        <v>253</v>
       </c>
       <c r="B34" s="4">
-        <v>255</v>
+        <v>95</v>
       </c>
       <c r="C34" s="3">
-        <v>43</v>
+        <v>247</v>
       </c>
       <c r="D34" s="4">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="E34" s="23"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="5">
-        <v>216</v>
+        <v>14</v>
       </c>
       <c r="B35" s="6">
-        <v>13</v>
+        <v>212</v>
       </c>
       <c r="C35" s="5">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="D35" s="6">
-        <v>17</v>
+        <v>139</v>
       </c>
       <c r="E35" s="23"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="B36" s="1">
-        <v>153</v>
+        <v>44</v>
       </c>
       <c r="C36" s="2">
-        <v>139</v>
+        <v>216</v>
       </c>
       <c r="D36" s="1">
-        <v>151</v>
+        <v>86</v>
       </c>
       <c r="E36" s="23"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="4">
-        <v>190</v>
+        <v>131</v>
       </c>
       <c r="B37" s="3">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="C37" s="4">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="D37" s="3">
-        <v>55</v>
+        <v>204</v>
       </c>
       <c r="E37" s="23"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="4">
-        <v>48</v>
+        <v>255</v>
       </c>
       <c r="B38" s="3">
-        <v>41</v>
+        <v>126</v>
       </c>
       <c r="C38" s="4">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="D38" s="3">
-        <v>81</v>
+        <v>221</v>
       </c>
       <c r="E38" s="23"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="4">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B39" s="3">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C39" s="4">
-        <v>208</v>
+        <v>161</v>
       </c>
       <c r="D39" s="3">
-        <v>216</v>
+        <v>39</v>
       </c>
       <c r="E39" s="23"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="6">
-        <v>129</v>
+        <v>28</v>
       </c>
       <c r="B40" s="5">
-        <v>98</v>
+        <v>205</v>
       </c>
       <c r="C40" s="6">
-        <v>143</v>
+        <v>34</v>
       </c>
       <c r="D40" s="5">
-        <v>185</v>
+        <v>110</v>
       </c>
       <c r="E40" s="23"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="7">
-        <v>220</v>
+        <v>177</v>
       </c>
       <c r="B41" s="8">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="C41" s="7">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="D41" s="8">
-        <v>33</v>
+        <v>207</v>
       </c>
       <c r="E41" s="23" t="s">
         <v>2</v>
@@ -1337,301 +1337,301 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="9">
-        <v>231</v>
+        <v>209</v>
       </c>
       <c r="B42" s="10">
-        <v>65</v>
+        <v>139</v>
       </c>
       <c r="C42" s="9">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="D42" s="10">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E42" s="23"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="9">
-        <v>200</v>
+        <v>156</v>
       </c>
       <c r="B43" s="10">
-        <v>96</v>
+        <v>21</v>
       </c>
       <c r="C43" s="9">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="D43" s="10">
-        <v>209</v>
+        <v>161</v>
       </c>
       <c r="E43" s="23"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="9">
-        <v>201</v>
+        <v>170</v>
       </c>
       <c r="B44" s="10">
-        <v>46</v>
+        <v>193</v>
       </c>
       <c r="C44" s="9">
-        <v>61</v>
+        <v>233</v>
       </c>
       <c r="D44" s="10">
-        <v>145</v>
+        <v>197</v>
       </c>
       <c r="E44" s="23"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="B45" s="12">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="C45" s="11">
-        <v>122</v>
+        <v>223</v>
       </c>
       <c r="D45" s="12">
-        <v>145</v>
+        <v>48</v>
       </c>
       <c r="E45" s="23"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="8">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="B46" s="7">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="C46" s="8">
-        <v>210</v>
+        <v>99</v>
       </c>
       <c r="D46" s="7">
-        <v>135</v>
+        <v>15</v>
       </c>
       <c r="E46" s="23"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="10">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="B47" s="9">
-        <v>137</v>
+        <v>182</v>
       </c>
       <c r="C47" s="10">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="D47" s="9">
-        <v>96</v>
+        <v>180</v>
       </c>
       <c r="E47" s="23"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="10">
-        <v>251</v>
+        <v>47</v>
       </c>
       <c r="B48" s="9">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="C48" s="10">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="D48" s="9">
-        <v>118</v>
+        <v>55</v>
       </c>
       <c r="E48" s="23"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="10">
-        <v>43</v>
+        <v>159</v>
       </c>
       <c r="B49" s="9">
-        <v>178</v>
+        <v>20</v>
       </c>
       <c r="C49" s="10">
-        <v>229</v>
+        <v>114</v>
       </c>
       <c r="D49" s="9">
-        <v>17</v>
+        <v>205</v>
       </c>
       <c r="E49" s="23"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="12">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="B50" s="11">
         <v>4</v>
       </c>
       <c r="C50" s="12">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D50" s="11">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="E50" s="23"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="7">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="B51" s="8">
-        <v>193</v>
+        <v>158</v>
       </c>
       <c r="C51" s="7">
-        <v>36</v>
+        <v>170</v>
       </c>
       <c r="D51" s="8">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="E51" s="23"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="9">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="B52" s="10">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="C52" s="9">
-        <v>81</v>
+        <v>146</v>
       </c>
       <c r="D52" s="10">
-        <v>202</v>
+        <v>10</v>
       </c>
       <c r="E52" s="23"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="9">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="B53" s="10">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C53" s="9">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="D53" s="10">
-        <v>216</v>
+        <v>251</v>
       </c>
       <c r="E53" s="23"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="9">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B54" s="10">
-        <v>244</v>
+        <v>88</v>
       </c>
       <c r="C54" s="9">
-        <v>208</v>
+        <v>116</v>
       </c>
       <c r="D54" s="10">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="E54" s="23"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="11">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B55" s="12">
-        <v>163</v>
+        <v>195</v>
       </c>
       <c r="C55" s="11">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="D55" s="12">
-        <v>119</v>
+        <v>16</v>
       </c>
       <c r="E55" s="23"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="8">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="B56" s="7">
-        <v>18</v>
+        <v>216</v>
       </c>
       <c r="C56" s="8">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D56" s="7">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="E56" s="23"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="10">
-        <v>234</v>
+        <v>152</v>
       </c>
       <c r="B57" s="9">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C57" s="10">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D57" s="9">
-        <v>255</v>
+        <v>181</v>
       </c>
       <c r="E57" s="23"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="10">
-        <v>124</v>
+        <v>247</v>
       </c>
       <c r="B58" s="9">
-        <v>158</v>
+        <v>188</v>
       </c>
       <c r="C58" s="10">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="D58" s="9">
-        <v>165</v>
+        <v>3</v>
       </c>
       <c r="E58" s="23"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="10">
-        <v>52</v>
+        <v>174</v>
       </c>
       <c r="B59" s="9">
-        <v>196</v>
+        <v>154</v>
       </c>
       <c r="C59" s="10">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D59" s="9">
-        <v>201</v>
+        <v>38</v>
       </c>
       <c r="E59" s="23"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="12">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B60" s="11">
-        <v>58</v>
+        <v>204</v>
       </c>
       <c r="C60" s="12">
-        <v>34</v>
+        <v>117</v>
       </c>
       <c r="D60" s="11">
-        <v>209</v>
+        <v>64</v>
       </c>
       <c r="E60" s="23"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="7">
-        <v>244</v>
+        <v>20</v>
       </c>
       <c r="B61" s="8">
-        <v>138</v>
+        <v>72</v>
       </c>
       <c r="C61" s="7">
-        <v>16</v>
+        <v>188</v>
       </c>
       <c r="D61" s="8">
-        <v>164</v>
+        <v>207</v>
       </c>
       <c r="E61" s="23" t="s">
         <v>3</v>
@@ -1639,791 +1639,791 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="9">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="B62" s="10">
-        <v>205</v>
+        <v>67</v>
       </c>
       <c r="C62" s="9">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="D62" s="10">
-        <v>180</v>
+        <v>112</v>
       </c>
       <c r="E62" s="23"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="9">
-        <v>239</v>
+        <v>155</v>
       </c>
       <c r="B63" s="10">
-        <v>228</v>
+        <v>61</v>
       </c>
       <c r="C63" s="9">
-        <v>149</v>
+        <v>94</v>
       </c>
       <c r="D63" s="10">
-        <v>105</v>
+        <v>182</v>
       </c>
       <c r="E63" s="23"/>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="9">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B64" s="10">
-        <v>71</v>
+        <v>215</v>
       </c>
       <c r="C64" s="9">
-        <v>12</v>
+        <v>184</v>
       </c>
       <c r="D64" s="10">
-        <v>166</v>
+        <v>103</v>
       </c>
       <c r="E64" s="23"/>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="11">
-        <v>251</v>
+        <v>169</v>
       </c>
       <c r="B65" s="12">
-        <v>84</v>
+        <v>204</v>
       </c>
       <c r="C65" s="11">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="D65" s="12">
-        <v>136</v>
+        <v>245</v>
       </c>
       <c r="E65" s="23"/>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="8">
-        <v>132</v>
+        <v>65</v>
       </c>
       <c r="B66" s="7">
-        <v>243</v>
+        <v>183</v>
       </c>
       <c r="C66" s="8">
-        <v>171</v>
+        <v>217</v>
       </c>
       <c r="D66" s="7">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="E66" s="23"/>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="10">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="B67" s="9">
-        <v>102</v>
+        <v>228</v>
       </c>
       <c r="C67" s="10">
-        <v>112</v>
+        <v>218</v>
       </c>
       <c r="D67" s="9">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E67" s="23"/>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="10">
-        <v>229</v>
+        <v>79</v>
       </c>
       <c r="B68" s="9">
-        <v>9</v>
+        <v>225</v>
       </c>
       <c r="C68" s="10">
-        <v>18</v>
+        <v>234</v>
       </c>
       <c r="D68" s="9">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="E68" s="23"/>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="10">
-        <v>248</v>
+        <v>65</v>
       </c>
       <c r="B69" s="9">
-        <v>152</v>
+        <v>246</v>
       </c>
       <c r="C69" s="10">
-        <v>191</v>
+        <v>93</v>
       </c>
       <c r="D69" s="9">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="E69" s="23"/>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="12">
-        <v>95</v>
+        <v>39</v>
       </c>
       <c r="B70" s="11">
-        <v>232</v>
+        <v>206</v>
       </c>
       <c r="C70" s="12">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="D70" s="11">
-        <v>236</v>
+        <v>166</v>
       </c>
       <c r="E70" s="23"/>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="7">
-        <v>188</v>
+        <v>111</v>
       </c>
       <c r="B71" s="8">
-        <v>60</v>
+        <v>213</v>
       </c>
       <c r="C71" s="7">
-        <v>228</v>
+        <v>189</v>
       </c>
       <c r="D71" s="8">
-        <v>172</v>
+        <v>95</v>
       </c>
       <c r="E71" s="23"/>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="9">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="B72" s="10">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="C72" s="9">
-        <v>247</v>
+        <v>28</v>
       </c>
       <c r="D72" s="10">
-        <v>226</v>
+        <v>113</v>
       </c>
       <c r="E72" s="23"/>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="9">
-        <v>19</v>
+        <v>155</v>
       </c>
       <c r="B73" s="10">
-        <v>240</v>
+        <v>70</v>
       </c>
       <c r="C73" s="9">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D73" s="10">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="E73" s="23"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="9">
-        <v>142</v>
+        <v>53</v>
       </c>
       <c r="B74" s="10">
-        <v>126</v>
+        <v>193</v>
       </c>
       <c r="C74" s="9">
-        <v>193</v>
+        <v>89</v>
       </c>
       <c r="D74" s="10">
-        <v>73</v>
+        <v>112</v>
       </c>
       <c r="E74" s="23"/>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="11">
-        <v>33</v>
+        <v>169</v>
       </c>
       <c r="B75" s="12">
-        <v>4</v>
+        <v>229</v>
       </c>
       <c r="C75" s="11">
-        <v>160</v>
+        <v>108</v>
       </c>
       <c r="D75" s="12">
-        <v>112</v>
+        <v>156</v>
       </c>
       <c r="E75" s="23"/>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="8">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B76" s="7">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C76" s="8">
-        <v>51</v>
+        <v>112</v>
       </c>
       <c r="D76" s="7">
-        <v>13</v>
+        <v>225</v>
       </c>
       <c r="E76" s="23"/>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="10">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="B77" s="9">
-        <v>217</v>
+        <v>52</v>
       </c>
       <c r="C77" s="10">
-        <v>61</v>
+        <v>250</v>
       </c>
       <c r="D77" s="9">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="E77" s="23"/>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="10">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="B78" s="9">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="C78" s="10">
-        <v>3</v>
+        <v>209</v>
       </c>
       <c r="D78" s="9">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="E78" s="23"/>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="10">
-        <v>18</v>
+        <v>212</v>
       </c>
       <c r="B79" s="9">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="C79" s="10">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="D79" s="9">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="E79" s="23"/>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="12">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B80" s="11">
-        <v>30</v>
+        <v>246</v>
       </c>
       <c r="C80" s="12">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D80" s="11">
-        <v>131</v>
+        <v>76</v>
       </c>
       <c r="E80" s="23"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="13">
-        <v>93</v>
+        <v>164</v>
       </c>
       <c r="B81" s="14">
-        <v>172</v>
+        <v>0</v>
       </c>
       <c r="C81" s="13">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="D81" s="14">
-        <v>131</v>
+        <v>189</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="15">
-        <v>165</v>
+        <v>18</v>
       </c>
       <c r="B82" s="16">
-        <v>113</v>
+        <v>236</v>
       </c>
       <c r="C82" s="15">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="D82" s="16">
-        <v>64</v>
+        <v>112</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="15">
-        <v>239</v>
+        <v>27</v>
       </c>
       <c r="B83" s="16">
-        <v>243</v>
+        <v>118</v>
       </c>
       <c r="C83" s="15">
+        <v>107</v>
+      </c>
+      <c r="D83" s="16">
         <v>25</v>
-      </c>
-      <c r="D83" s="16">
-        <v>240</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="15">
-        <v>167</v>
+        <v>202</v>
       </c>
       <c r="B84" s="16">
-        <v>140</v>
+        <v>86</v>
       </c>
       <c r="C84" s="15">
-        <v>28</v>
+        <v>102</v>
       </c>
       <c r="D84" s="16">
-        <v>92</v>
+        <v>44</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="15">
-        <v>55</v>
+        <v>189</v>
       </c>
       <c r="B85" s="16">
-        <v>226</v>
+        <v>106</v>
       </c>
       <c r="C85" s="15">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="D85" s="16">
-        <v>32</v>
+        <v>90</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="15">
-        <v>129</v>
+        <v>193</v>
       </c>
       <c r="B86" s="16">
-        <v>239</v>
+        <v>208</v>
       </c>
       <c r="C86" s="15">
-        <v>227</v>
+        <v>150</v>
       </c>
       <c r="D86" s="16">
-        <v>194</v>
+        <v>31</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="15">
-        <v>36</v>
+        <v>137</v>
       </c>
       <c r="B87" s="16">
-        <v>203</v>
+        <v>152</v>
       </c>
       <c r="C87" s="15">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="D87" s="16">
-        <v>49</v>
+        <v>191</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="15">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B88" s="16">
-        <v>100</v>
+        <v>159</v>
       </c>
       <c r="C88" s="15">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D88" s="16">
-        <v>117</v>
+        <v>48</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="17">
-        <v>164</v>
+        <v>68</v>
       </c>
       <c r="B89" s="18">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="C89" s="17">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D89" s="18">
-        <v>189</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="14">
-        <v>216</v>
+        <v>178</v>
       </c>
       <c r="B90" s="13">
-        <v>190</v>
+        <v>218</v>
       </c>
       <c r="C90" s="14">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="D90" s="13">
-        <v>34</v>
+        <v>165</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="16">
-        <v>107</v>
+        <v>239</v>
       </c>
       <c r="B91" s="15">
-        <v>143</v>
+        <v>58</v>
       </c>
       <c r="C91" s="16">
-        <v>85</v>
+        <v>252</v>
       </c>
       <c r="D91" s="15">
-        <v>216</v>
+        <v>110</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="16">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="B92" s="15">
-        <v>14</v>
+        <v>126</v>
       </c>
       <c r="C92" s="16">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="D92" s="15">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="16">
-        <v>44</v>
+        <v>185</v>
       </c>
       <c r="B93" s="15">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="C93" s="16">
-        <v>245</v>
+        <v>56</v>
       </c>
       <c r="D93" s="15">
-        <v>59</v>
+        <v>145</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="16">
-        <v>65</v>
+        <v>149</v>
       </c>
       <c r="B94" s="15">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="C94" s="16">
-        <v>121</v>
+        <v>191</v>
       </c>
       <c r="D94" s="15">
-        <v>221</v>
+        <v>137</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="16">
-        <v>111</v>
+        <v>15</v>
       </c>
       <c r="B95" s="15">
-        <v>102</v>
+        <v>189</v>
       </c>
       <c r="C95" s="16">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="D95" s="15">
-        <v>186</v>
+        <v>38</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="16">
-        <v>231</v>
+        <v>129</v>
       </c>
       <c r="B96" s="15">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="C96" s="16">
-        <v>18</v>
+        <v>158</v>
       </c>
       <c r="D96" s="15">
-        <v>106</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="16">
-        <v>229</v>
+        <v>24</v>
       </c>
       <c r="B97" s="15">
-        <v>48</v>
+        <v>232</v>
       </c>
       <c r="C97" s="16">
-        <v>195</v>
+        <v>162</v>
       </c>
       <c r="D97" s="15">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="18">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B98" s="17">
-        <v>218</v>
+        <v>160</v>
       </c>
       <c r="C98" s="18">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="D98" s="17">
-        <v>165</v>
+        <v>253</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="13">
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="B99" s="14">
-        <v>193</v>
+        <v>108</v>
       </c>
       <c r="C99" s="13">
-        <v>157</v>
+        <v>228</v>
       </c>
       <c r="D99" s="14">
-        <v>153</v>
+        <v>46</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="15">
-        <v>181</v>
+        <v>117</v>
       </c>
       <c r="B100" s="16">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C100" s="15">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="D100" s="16">
-        <v>24</v>
+        <v>213</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="15">
-        <v>35</v>
+        <v>114</v>
       </c>
       <c r="B101" s="16">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="C101" s="15">
-        <v>94</v>
+        <v>242</v>
       </c>
       <c r="D101" s="16">
-        <v>168</v>
+        <v>22</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="15">
-        <v>39</v>
+        <v>126</v>
       </c>
       <c r="B102" s="16">
-        <v>193</v>
+        <v>74</v>
       </c>
       <c r="C102" s="15">
-        <v>235</v>
+        <v>73</v>
       </c>
       <c r="D102" s="16">
-        <v>98</v>
+        <v>18</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="15">
-        <v>228</v>
+        <v>75</v>
       </c>
       <c r="B103" s="16">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="C103" s="15">
-        <v>152</v>
+        <v>179</v>
       </c>
       <c r="D103" s="16">
-        <v>188</v>
+        <v>33</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="15">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="B104" s="16">
-        <v>134</v>
+        <v>204</v>
       </c>
       <c r="C104" s="15">
-        <v>137</v>
+        <v>217</v>
       </c>
       <c r="D104" s="16">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="15">
-        <v>84</v>
+        <v>236</v>
       </c>
       <c r="B105" s="16">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="C105" s="15">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="D105" s="16">
-        <v>24</v>
+        <v>191</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="15">
-        <v>69</v>
+        <v>211</v>
       </c>
       <c r="B106" s="16">
-        <v>144</v>
+        <v>98</v>
       </c>
       <c r="C106" s="15">
-        <v>176</v>
+        <v>88</v>
       </c>
       <c r="D106" s="16">
-        <v>170</v>
+        <v>181</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="17">
-        <v>212</v>
+        <v>70</v>
       </c>
       <c r="B107" s="18">
-        <v>108</v>
+        <v>31</v>
       </c>
       <c r="C107" s="17">
-        <v>228</v>
+        <v>141</v>
       </c>
       <c r="D107" s="18">
-        <v>46</v>
+        <v>112</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="14">
-        <v>9</v>
+        <v>233</v>
       </c>
       <c r="B108" s="13">
-        <v>3</v>
+        <v>131</v>
       </c>
       <c r="C108" s="14">
-        <v>175</v>
+        <v>242</v>
       </c>
       <c r="D108" s="13">
-        <v>179</v>
+        <v>82</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="16">
-        <v>180</v>
+        <v>27</v>
       </c>
       <c r="B109" s="15">
-        <v>175</v>
+        <v>230</v>
       </c>
       <c r="C109" s="16">
-        <v>73</v>
+        <v>218</v>
       </c>
       <c r="D109" s="15">
-        <v>54</v>
+        <v>96</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="16">
-        <v>46</v>
+        <v>141</v>
       </c>
       <c r="B110" s="15">
-        <v>173</v>
+        <v>252</v>
       </c>
       <c r="C110" s="16">
-        <v>141</v>
+        <v>89</v>
       </c>
       <c r="D110" s="15">
-        <v>10</v>
+        <v>88</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="16">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="B111" s="15">
-        <v>195</v>
+        <v>254</v>
       </c>
       <c r="C111" s="16">
-        <v>19</v>
+        <v>236</v>
       </c>
       <c r="D111" s="15">
-        <v>112</v>
+        <v>87</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="16">
-        <v>72</v>
+        <v>16</v>
       </c>
       <c r="B112" s="15">
-        <v>232</v>
+        <v>57</v>
       </c>
       <c r="C112" s="16">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="D112" s="15">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="16">
-        <v>113</v>
+        <v>70</v>
       </c>
       <c r="B113" s="15">
-        <v>227</v>
+        <v>32</v>
       </c>
       <c r="C113" s="16">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="D113" s="15">
-        <v>217</v>
+        <v>33</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="16">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="B114" s="15">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C114" s="16">
-        <v>111</v>
+        <v>11</v>
       </c>
       <c r="D114" s="15">
-        <v>152</v>
+        <v>238</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="16">
-        <v>76</v>
+        <v>250</v>
       </c>
       <c r="B115" s="15">
-        <v>239</v>
+        <v>191</v>
       </c>
       <c r="C115" s="16">
-        <v>135</v>
+        <v>81</v>
       </c>
       <c r="D115" s="15">
-        <v>18</v>
+        <v>125</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="18">
-        <v>233</v>
+        <v>204</v>
       </c>
       <c r="B116" s="17">
-        <v>131</v>
+        <v>26</v>
       </c>
       <c r="C116" s="18">
-        <v>242</v>
+        <v>124</v>
       </c>
       <c r="D116" s="17">
-        <v>82</v>
+        <v>218</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2624,28 +2624,28 @@
     <row r="1" spans="1:10">
       <c r="A1" s="19">
         <f>Foglio1!A1*Foglio1!A81</f>
-        <v>7440</v>
+        <v>23944</v>
       </c>
       <c r="B1" s="19">
         <f>Foglio1!B1*Foglio1!B81</f>
-        <v>20812</v>
+        <v>0</v>
       </c>
       <c r="C1" s="19">
         <f>Foglio1!C1*Foglio1!C81</f>
-        <v>36890</v>
+        <v>0</v>
       </c>
       <c r="D1" s="19">
         <f>Foglio1!D1*Foglio1!D81</f>
-        <v>28820</v>
+        <v>41958</v>
       </c>
       <c r="E1" s="24"/>
       <c r="F1">
         <f>SUM(A1:D1)</f>
-        <v>93962</v>
+        <v>65902</v>
       </c>
       <c r="I1">
         <f>F1+F6+F11+F16</f>
-        <v>313094</v>
+        <v>299587</v>
       </c>
       <c r="J1" t="e">
         <f>DEC2BIN(I1,32)</f>
@@ -2655,28 +2655,28 @@
     <row r="2" spans="1:10">
       <c r="A2" s="19">
         <f>Foglio1!A2*Foglio1!A82</f>
-        <v>13695</v>
+        <v>3564</v>
       </c>
       <c r="B2" s="19">
         <f>Foglio1!B2*Foglio1!B82</f>
-        <v>24521</v>
+        <v>23836</v>
       </c>
       <c r="C2" s="19">
         <f>Foglio1!C2*Foglio1!C82</f>
-        <v>37399</v>
+        <v>11664</v>
       </c>
       <c r="D2" s="19">
         <f>Foglio1!D2*Foglio1!D82</f>
-        <v>640</v>
+        <v>28448</v>
       </c>
       <c r="E2" s="24"/>
       <c r="F2">
         <f t="shared" ref="F2:F20" si="0">SUM(A2:D2)</f>
-        <v>76255</v>
+        <v>67512</v>
       </c>
       <c r="I2">
         <f>F2+F7+F12+F17</f>
-        <v>257372</v>
+        <v>284190</v>
       </c>
       <c r="J2" t="e">
         <f>DEC2BIN(I2,32)</f>
@@ -2686,1387 +2686,1387 @@
     <row r="3" spans="1:10">
       <c r="A3" s="19">
         <f>Foglio1!A3*Foglio1!A83</f>
-        <v>11950</v>
+        <v>4833</v>
       </c>
       <c r="B3" s="19">
         <f>Foglio1!B3*Foglio1!B83</f>
-        <v>10449</v>
+        <v>17464</v>
       </c>
       <c r="C3" s="19">
         <f>Foglio1!C3*Foglio1!C83</f>
-        <v>2675</v>
+        <v>25252</v>
       </c>
       <c r="D3" s="19">
         <f>Foglio1!D3*Foglio1!D83</f>
-        <v>39360</v>
+        <v>4075</v>
       </c>
       <c r="E3" s="24"/>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>64434</v>
+        <v>51624</v>
       </c>
       <c r="I3">
         <f>F3+F8+F13+F18</f>
-        <v>141751</v>
+        <v>216438</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="19">
         <f>Foglio1!A4*Foglio1!A84</f>
-        <v>5344</v>
+        <v>28684</v>
       </c>
       <c r="B4" s="19">
         <f>Foglio1!B4*Foglio1!B84</f>
-        <v>14140</v>
+        <v>19006</v>
       </c>
       <c r="C4" s="19">
         <f>Foglio1!C4*Foglio1!C84</f>
-        <v>2548</v>
+        <v>16320</v>
       </c>
       <c r="D4" s="19">
         <f>Foglio1!D4*Foglio1!D84</f>
-        <v>1288</v>
+        <v>3828</v>
       </c>
       <c r="E4" s="24"/>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>23320</v>
+        <v>67838</v>
       </c>
       <c r="I4">
         <f>F4+F9+F14+F19</f>
-        <v>174687</v>
+        <v>292303</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="19">
         <f>Foglio1!A5*Foglio1!A85</f>
-        <v>13365</v>
+        <v>39501</v>
       </c>
       <c r="B5" s="19">
         <f>Foglio1!B5*Foglio1!B85</f>
-        <v>17628</v>
+        <v>19504</v>
       </c>
       <c r="C5" s="19">
         <f>Foglio1!C5*Foglio1!C85</f>
-        <v>19836</v>
+        <v>8003</v>
       </c>
       <c r="D5" s="19">
         <f>Foglio1!D5*Foglio1!D85</f>
-        <v>4192</v>
+        <v>90</v>
       </c>
       <c r="E5" s="24"/>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>55021</v>
+        <v>67098</v>
       </c>
       <c r="I5">
         <f>F5+F10+F15+F20</f>
-        <v>270020</v>
+        <v>184048</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="20">
         <f>Foglio1!A6*Foglio1!A90</f>
-        <v>3888</v>
+        <v>33998</v>
       </c>
       <c r="B6" s="20">
         <f>Foglio1!B6*Foglio1!B90</f>
-        <v>48450</v>
+        <v>17440</v>
       </c>
       <c r="C6" s="20">
         <f>Foglio1!C6*Foglio1!C90</f>
-        <v>756</v>
+        <v>7410</v>
       </c>
       <c r="D6" s="20">
         <f>Foglio1!D6*Foglio1!D90</f>
-        <v>6596</v>
+        <v>28710</v>
       </c>
       <c r="E6" s="24"/>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>59690</v>
+        <v>87558</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="20">
         <f>Foglio1!A7*Foglio1!A91</f>
-        <v>14552</v>
+        <v>40152</v>
       </c>
       <c r="B7" s="20">
         <f>Foglio1!B7*Foglio1!B91</f>
-        <v>1716</v>
+        <v>8352</v>
       </c>
       <c r="C7" s="20">
         <f>Foglio1!C7*Foglio1!C91</f>
-        <v>14365</v>
+        <v>21168</v>
       </c>
       <c r="D7" s="20">
         <f>Foglio1!D7*Foglio1!D91</f>
-        <v>37800</v>
+        <v>24640</v>
       </c>
       <c r="E7" s="24"/>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>68433</v>
+        <v>94312</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="20">
         <f>Foglio1!A8*Foglio1!A92</f>
-        <v>3872</v>
+        <v>9065</v>
       </c>
       <c r="B8" s="20">
         <f>Foglio1!B8*Foglio1!B92</f>
-        <v>3458</v>
+        <v>3402</v>
       </c>
       <c r="C8" s="20">
         <f>Foglio1!C8*Foglio1!C92</f>
-        <v>16352</v>
+        <v>744</v>
       </c>
       <c r="D8" s="20">
         <f>Foglio1!D8*Foglio1!D92</f>
-        <v>3894</v>
+        <v>11937</v>
       </c>
       <c r="E8" s="24"/>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>27576</v>
+        <v>25148</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="20">
         <f>Foglio1!A9*Foglio1!A93</f>
-        <v>10780</v>
+        <v>3700</v>
       </c>
       <c r="B9" s="20">
         <f>Foglio1!B9*Foglio1!B93</f>
-        <v>21320</v>
+        <v>4797</v>
       </c>
       <c r="C9" s="20">
         <f>Foglio1!C9*Foglio1!C93</f>
-        <v>17395</v>
+        <v>672</v>
       </c>
       <c r="D9" s="20">
         <f>Foglio1!D9*Foglio1!D93</f>
-        <v>11859</v>
+        <v>36395</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>61354</v>
+        <v>45564</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="20">
         <f>Foglio1!A10*Foglio1!A94</f>
-        <v>9230</v>
+        <v>28906</v>
       </c>
       <c r="B10" s="20">
         <f>Foglio1!B10*Foglio1!B94</f>
-        <v>8729</v>
+        <v>0</v>
       </c>
       <c r="C10" s="20">
         <f>Foglio1!C10*Foglio1!C94</f>
-        <v>22869</v>
+        <v>4393</v>
       </c>
       <c r="D10" s="20">
         <f>Foglio1!D10*Foglio1!D94</f>
-        <v>1768</v>
+        <v>26852</v>
       </c>
       <c r="E10" s="24"/>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>42596</v>
+        <v>60151</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="19">
         <f>Foglio1!A11*Foglio1!A99</f>
-        <v>36432</v>
+        <v>27560</v>
       </c>
       <c r="B11" s="19">
         <f>Foglio1!B11*Foglio1!B99</f>
-        <v>11580</v>
+        <v>13392</v>
       </c>
       <c r="C11" s="19">
         <f>Foglio1!C11*Foglio1!C99</f>
-        <v>39407</v>
+        <v>52212</v>
       </c>
       <c r="D11" s="19">
         <f>Foglio1!D11*Foglio1!D99</f>
-        <v>13464</v>
+        <v>2852</v>
       </c>
       <c r="E11" s="24"/>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>100883</v>
+        <v>96016</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="19">
         <f>Foglio1!A12*Foglio1!A100</f>
-        <v>31494</v>
+        <v>25857</v>
       </c>
       <c r="B12" s="19">
         <f>Foglio1!B12*Foglio1!B100</f>
-        <v>31</v>
+        <v>924</v>
       </c>
       <c r="C12" s="19">
         <f>Foglio1!C12*Foglio1!C100</f>
-        <v>18070</v>
+        <v>4515</v>
       </c>
       <c r="D12" s="19">
         <f>Foglio1!D12*Foglio1!D100</f>
-        <v>4800</v>
+        <v>10650</v>
       </c>
       <c r="E12" s="24"/>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>54395</v>
+        <v>41946</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="19">
         <f>Foglio1!A13*Foglio1!A101</f>
-        <v>2345</v>
+        <v>23826</v>
       </c>
       <c r="B13" s="19">
         <f>Foglio1!B13*Foglio1!B101</f>
-        <v>12905</v>
+        <v>6302</v>
       </c>
       <c r="C13" s="19">
         <f>Foglio1!C13*Foglio1!C101</f>
-        <v>1316</v>
+        <v>33638</v>
       </c>
       <c r="D13" s="19">
         <f>Foglio1!D13*Foglio1!D101</f>
-        <v>22176</v>
+        <v>2596</v>
       </c>
       <c r="E13" s="24"/>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>38742</v>
+        <v>66362</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="19">
         <f>Foglio1!A14*Foglio1!A102</f>
-        <v>702</v>
+        <v>30492</v>
       </c>
       <c r="B14" s="19">
         <f>Foglio1!B14*Foglio1!B102</f>
-        <v>38214</v>
+        <v>11470</v>
       </c>
       <c r="C14" s="19">
         <f>Foglio1!C14*Foglio1!C102</f>
-        <v>17390</v>
+        <v>8103</v>
       </c>
       <c r="D14" s="19">
         <f>Foglio1!D14*Foglio1!D102</f>
-        <v>1666</v>
+        <v>4446</v>
       </c>
       <c r="E14" s="24"/>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>57972</v>
+        <v>54511</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="19">
         <f>Foglio1!A15*Foglio1!A103</f>
-        <v>46284</v>
+        <v>18075</v>
       </c>
       <c r="B15" s="19">
         <f>Foglio1!B15*Foglio1!B103</f>
-        <v>14278</v>
+        <v>1120</v>
       </c>
       <c r="C15" s="19">
         <f>Foglio1!C15*Foglio1!C103</f>
-        <v>18392</v>
+        <v>895</v>
       </c>
       <c r="D15" s="19">
         <f>Foglio1!D15*Foglio1!D103</f>
-        <v>30832</v>
+        <v>5346</v>
       </c>
       <c r="E15" s="24"/>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>109786</v>
+        <v>25436</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="20">
         <f>Foglio1!A16*Foglio1!A108</f>
-        <v>675</v>
+        <v>20970</v>
       </c>
       <c r="B16" s="20">
         <f>Foglio1!B16*Foglio1!B108</f>
-        <v>252</v>
+        <v>18995</v>
       </c>
       <c r="C16" s="20">
         <f>Foglio1!C16*Foglio1!C108</f>
-        <v>15925</v>
+        <v>6292</v>
       </c>
       <c r="D16" s="20">
         <f>Foglio1!D16*Foglio1!D108</f>
-        <v>41707</v>
+        <v>3854</v>
       </c>
       <c r="E16" s="24"/>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>58559</v>
+        <v>50111</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="20">
         <f>Foglio1!A17*Foglio1!A109</f>
-        <v>8280</v>
+        <v>2862</v>
       </c>
       <c r="B17" s="20">
         <f>Foglio1!B17*Foglio1!B109</f>
-        <v>32200</v>
+        <v>43470</v>
       </c>
       <c r="C17" s="20">
         <f>Foglio1!C17*Foglio1!C109</f>
-        <v>5767</v>
+        <v>11336</v>
       </c>
       <c r="D17" s="20">
         <f>Foglio1!D17*Foglio1!D109</f>
-        <v>12042</v>
+        <v>22752</v>
       </c>
       <c r="E17" s="24"/>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>58289</v>
+        <v>80420</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="20">
         <f>Foglio1!A18*Foglio1!A110</f>
-        <v>8786</v>
+        <v>29046</v>
       </c>
       <c r="B18" s="20">
         <f>Foglio1!B18*Foglio1!B110</f>
-        <v>1038</v>
+        <v>23436</v>
       </c>
       <c r="C18" s="20">
         <f>Foglio1!C18*Foglio1!C110</f>
-        <v>705</v>
+        <v>12638</v>
       </c>
       <c r="D18" s="20">
         <f>Foglio1!D18*Foglio1!D110</f>
-        <v>470</v>
+        <v>8184</v>
       </c>
       <c r="E18" s="24"/>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>10999</v>
+        <v>73304</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="20">
         <f>Foglio1!A19*Foglio1!A111</f>
-        <v>17466</v>
+        <v>62744</v>
       </c>
       <c r="B19" s="20">
         <f>Foglio1!B19*Foglio1!B111</f>
-        <v>1950</v>
+        <v>1270</v>
       </c>
       <c r="C19" s="20">
         <f>Foglio1!C19*Foglio1!C111</f>
-        <v>1425</v>
+        <v>44368</v>
       </c>
       <c r="D19" s="20">
         <f>Foglio1!D19*Foglio1!D111</f>
-        <v>11200</v>
+        <v>16008</v>
       </c>
       <c r="E19" s="24"/>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>32041</v>
+        <v>124390</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="20">
         <f>Foglio1!A20*Foglio1!A112</f>
-        <v>10152</v>
+        <v>16</v>
       </c>
       <c r="B20" s="20">
         <f>Foglio1!B20*Foglio1!B112</f>
-        <v>47560</v>
+        <v>13908</v>
       </c>
       <c r="C20" s="20">
         <f>Foglio1!C20*Foglio1!C112</f>
-        <v>174</v>
+        <v>9044</v>
       </c>
       <c r="D20" s="20">
         <f>Foglio1!D20*Foglio1!D112</f>
-        <v>4731</v>
+        <v>8395</v>
       </c>
       <c r="E20" s="24"/>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>62617</v>
+        <v>31363</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="19">
         <f>Foglio1!A21*Foglio1!A81</f>
-        <v>16275</v>
+        <v>4756</v>
       </c>
       <c r="B21" s="19">
         <f>Foglio1!B21*Foglio1!B81</f>
-        <v>12040</v>
+        <v>0</v>
       </c>
       <c r="C21" s="19">
         <f>Foglio1!C21*Foglio1!C81</f>
-        <v>6355</v>
+        <v>0</v>
       </c>
       <c r="D21" s="19">
         <f>Foglio1!D21*Foglio1!D81</f>
-        <v>26200</v>
+        <v>19656</v>
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="22">
         <f>SUM(A21:D21)</f>
-        <v>60870</v>
+        <v>24412</v>
       </c>
       <c r="G21" s="22">
         <f>F21+F26+F31+F36</f>
-        <v>215605</v>
+        <v>237646</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="19">
         <f>Foglio1!A22*Foglio1!A82</f>
-        <v>24090</v>
+        <v>3438</v>
       </c>
       <c r="B22" s="19">
         <f>Foglio1!B22*Foglio1!B82</f>
-        <v>12204</v>
+        <v>16284</v>
       </c>
       <c r="C22" s="19">
         <f>Foglio1!C22*Foglio1!C82</f>
-        <v>0</v>
+        <v>14364</v>
       </c>
       <c r="D22" s="19">
         <f>Foglio1!D22*Foglio1!D82</f>
-        <v>64</v>
+        <v>6384</v>
       </c>
       <c r="E22" s="26"/>
       <c r="F22">
         <f t="shared" ref="F22:F40" si="1">SUM(A22:D22)</f>
-        <v>36358</v>
+        <v>40470</v>
       </c>
       <c r="G22">
         <f t="shared" ref="G22:G25" si="2">F22+F27+F32+F37</f>
-        <v>269856</v>
+        <v>199764</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="19">
         <f>Foglio1!A23*Foglio1!A83</f>
-        <v>49473</v>
+        <v>1350</v>
       </c>
       <c r="B23" s="19">
         <f>Foglio1!B23*Foglio1!B83</f>
-        <v>23571</v>
+        <v>2124</v>
       </c>
       <c r="C23" s="19">
         <f>Foglio1!C23*Foglio1!C83</f>
-        <v>3525</v>
+        <v>19260</v>
       </c>
       <c r="D23" s="19">
         <f>Foglio1!D23*Foglio1!D83</f>
-        <v>56160</v>
+        <v>5650</v>
       </c>
       <c r="E23" s="26"/>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>132729</v>
+        <v>28384</v>
       </c>
       <c r="G23">
         <f t="shared" si="2"/>
-        <v>219938</v>
+        <v>201192</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="19">
         <f>Foglio1!A24*Foglio1!A84</f>
-        <v>30561</v>
+        <v>23028</v>
       </c>
       <c r="B24" s="19">
         <f>Foglio1!B24*Foglio1!B84</f>
-        <v>15400</v>
+        <v>4816</v>
       </c>
       <c r="C24" s="19">
         <f>Foglio1!C24*Foglio1!C84</f>
-        <v>5376</v>
+        <v>918</v>
       </c>
       <c r="D24" s="19">
         <f>Foglio1!D24*Foglio1!D84</f>
-        <v>2116</v>
+        <v>9240</v>
       </c>
       <c r="E24" s="26"/>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>53453</v>
+        <v>38002</v>
       </c>
       <c r="G24">
         <f t="shared" si="2"/>
-        <v>307046</v>
+        <v>324708</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="19">
         <f>Foglio1!A25*Foglio1!A85</f>
-        <v>8745</v>
+        <v>35154</v>
       </c>
       <c r="B25" s="19">
         <f>Foglio1!B25*Foglio1!B85</f>
-        <v>42488</v>
+        <v>6784</v>
       </c>
       <c r="C25" s="19">
         <f>Foglio1!C25*Foglio1!C85</f>
-        <v>7656</v>
+        <v>7852</v>
       </c>
       <c r="D25" s="19">
         <f>Foglio1!D25*Foglio1!D85</f>
-        <v>6240</v>
+        <v>20430</v>
       </c>
       <c r="E25" s="26"/>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>65129</v>
+        <v>70220</v>
       </c>
       <c r="G25">
         <f t="shared" si="2"/>
-        <v>256828</v>
+        <v>210786</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="20">
         <f>Foglio1!A26*Foglio1!A90</f>
-        <v>38880</v>
+        <v>22784</v>
       </c>
       <c r="B26" s="20">
         <f>Foglio1!B26*Foglio1!B90</f>
-        <v>4370</v>
+        <v>50358</v>
       </c>
       <c r="C26" s="20">
         <f>Foglio1!C26*Foglio1!C90</f>
-        <v>11256</v>
+        <v>7904</v>
       </c>
       <c r="D26" s="20">
         <f>Foglio1!D26*Foglio1!D90</f>
-        <v>5338</v>
+        <v>35310</v>
       </c>
       <c r="E26" s="26"/>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>59844</v>
+        <v>116356</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="20">
         <f>Foglio1!A27*Foglio1!A91</f>
-        <v>19153</v>
+        <v>0</v>
       </c>
       <c r="B27" s="20">
         <f>Foglio1!B27*Foglio1!B91</f>
-        <v>36179</v>
+        <v>3248</v>
       </c>
       <c r="C27" s="20">
         <f>Foglio1!C27*Foglio1!C91</f>
-        <v>10880</v>
+        <v>27468</v>
       </c>
       <c r="D27" s="20">
         <f>Foglio1!D27*Foglio1!D91</f>
-        <v>42552</v>
+        <v>19580</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27">
         <f t="shared" si="1"/>
-        <v>108764</v>
+        <v>50296</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="20">
         <f>Foglio1!A28*Foglio1!A92</f>
-        <v>0</v>
+        <v>2107</v>
       </c>
       <c r="B28" s="20">
         <f>Foglio1!B28*Foglio1!B92</f>
-        <v>742</v>
+        <v>756</v>
       </c>
       <c r="C28" s="20">
         <f>Foglio1!C28*Foglio1!C92</f>
-        <v>11680</v>
+        <v>2664</v>
       </c>
       <c r="D28" s="20">
         <f>Foglio1!D28*Foglio1!D92</f>
-        <v>660</v>
+        <v>7728</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>13082</v>
+        <v>13255</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="20">
         <f>Foglio1!A29*Foglio1!A93</f>
-        <v>1320</v>
+        <v>43660</v>
       </c>
       <c r="B29" s="20">
         <f>Foglio1!B29*Foglio1!B93</f>
-        <v>11752</v>
+        <v>21894</v>
       </c>
       <c r="C29" s="20">
         <f>Foglio1!C29*Foglio1!C93</f>
-        <v>59535</v>
+        <v>11088</v>
       </c>
       <c r="D29" s="20">
         <f>Foglio1!D29*Foglio1!D93</f>
-        <v>13098</v>
+        <v>31465</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29">
         <f t="shared" si="1"/>
-        <v>85705</v>
+        <v>108107</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="20">
         <f>Foglio1!A30*Foglio1!A94</f>
-        <v>15665</v>
+        <v>29055</v>
       </c>
       <c r="B30" s="20">
         <f>Foglio1!B30*Foglio1!B94</f>
-        <v>4128</v>
+        <v>0</v>
       </c>
       <c r="C30" s="20">
         <f>Foglio1!C30*Foglio1!C94</f>
-        <v>18513</v>
+        <v>42593</v>
       </c>
       <c r="D30" s="20">
         <f>Foglio1!D30*Foglio1!D94</f>
-        <v>35802</v>
+        <v>19865</v>
       </c>
       <c r="E30" s="26"/>
       <c r="F30">
         <f t="shared" si="1"/>
-        <v>74108</v>
+        <v>91513</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19">
         <f>Foglio1!A31*Foglio1!A99</f>
-        <v>9016</v>
+        <v>10176</v>
       </c>
       <c r="B31" s="19">
         <f>Foglio1!B31*Foglio1!B99</f>
-        <v>579</v>
+        <v>432</v>
       </c>
       <c r="C31" s="19">
         <f>Foglio1!C31*Foglio1!C99</f>
-        <v>471</v>
+        <v>3648</v>
       </c>
       <c r="D31" s="19">
         <f>Foglio1!D31*Foglio1!D99</f>
-        <v>32895</v>
+        <v>2622</v>
       </c>
       <c r="E31" s="26"/>
       <c r="F31">
         <f t="shared" si="1"/>
-        <v>42961</v>
+        <v>16878</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="19">
         <f>Foglio1!A32*Foglio1!A100</f>
-        <v>31494</v>
+        <v>24687</v>
       </c>
       <c r="B32" s="19">
         <f>Foglio1!B32*Foglio1!B100</f>
-        <v>252</v>
+        <v>2079</v>
       </c>
       <c r="C32" s="19">
         <f>Foglio1!C32*Foglio1!C100</f>
-        <v>25576</v>
+        <v>10815</v>
       </c>
       <c r="D32" s="19">
         <f>Foglio1!D32*Foglio1!D100</f>
-        <v>4512</v>
+        <v>25560</v>
       </c>
       <c r="E32" s="26"/>
       <c r="F32">
         <f t="shared" si="1"/>
-        <v>61834</v>
+        <v>63141</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19">
         <f>Foglio1!A33*Foglio1!A101</f>
-        <v>4375</v>
+        <v>28728</v>
       </c>
       <c r="B33" s="19">
         <f>Foglio1!B33*Foglio1!B101</f>
-        <v>3471</v>
+        <v>1840</v>
       </c>
       <c r="C33" s="19">
         <f>Foglio1!C33*Foglio1!C101</f>
-        <v>19270</v>
+        <v>21054</v>
       </c>
       <c r="D33" s="19">
         <f>Foglio1!D33*Foglio1!D101</f>
-        <v>5880</v>
+        <v>484</v>
       </c>
       <c r="E33" s="26"/>
       <c r="F33">
         <f t="shared" si="1"/>
-        <v>32996</v>
+        <v>52106</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19">
         <f>Foglio1!A34*Foglio1!A102</f>
-        <v>4368</v>
+        <v>31878</v>
       </c>
       <c r="B34" s="19">
         <f>Foglio1!B34*Foglio1!B102</f>
-        <v>49215</v>
+        <v>7030</v>
       </c>
       <c r="C34" s="19">
         <f>Foglio1!C34*Foglio1!C102</f>
-        <v>10105</v>
+        <v>18031</v>
       </c>
       <c r="D34" s="19">
         <f>Foglio1!D34*Foglio1!D102</f>
-        <v>3528</v>
+        <v>1260</v>
       </c>
       <c r="E34" s="26"/>
       <c r="F34">
         <f t="shared" si="1"/>
-        <v>67216</v>
+        <v>58199</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19">
         <f>Foglio1!A35*Foglio1!A103</f>
-        <v>49248</v>
+        <v>1050</v>
       </c>
       <c r="B35" s="19">
         <f>Foglio1!B35*Foglio1!B103</f>
-        <v>767</v>
+        <v>4240</v>
       </c>
       <c r="C35" s="19">
         <f>Foglio1!C35*Foglio1!C103</f>
-        <v>4560</v>
+        <v>17721</v>
       </c>
       <c r="D35" s="19">
         <f>Foglio1!D35*Foglio1!D103</f>
-        <v>3196</v>
+        <v>4587</v>
       </c>
       <c r="E35" s="26"/>
       <c r="F35">
         <f t="shared" si="1"/>
-        <v>57771</v>
+        <v>27598</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="20">
         <f>Foglio1!A36*Foglio1!A108</f>
-        <v>117</v>
+        <v>14912</v>
       </c>
       <c r="B36" s="20">
         <f>Foglio1!B36*Foglio1!B108</f>
-        <v>459</v>
+        <v>5764</v>
       </c>
       <c r="C36" s="20">
         <f>Foglio1!C36*Foglio1!C108</f>
-        <v>24325</v>
+        <v>52272</v>
       </c>
       <c r="D36" s="20">
         <f>Foglio1!D36*Foglio1!D108</f>
-        <v>27029</v>
+        <v>7052</v>
       </c>
       <c r="E36" s="26"/>
       <c r="F36">
         <f t="shared" si="1"/>
-        <v>51930</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="20">
         <f>Foglio1!A37*Foglio1!A109</f>
-        <v>34200</v>
+        <v>3537</v>
       </c>
       <c r="B37" s="20">
         <f>Foglio1!B37*Foglio1!B109</f>
-        <v>21350</v>
+        <v>17940</v>
       </c>
       <c r="C37" s="20">
         <f>Foglio1!C37*Foglio1!C109</f>
-        <v>4380</v>
+        <v>4796</v>
       </c>
       <c r="D37" s="20">
         <f>Foglio1!D37*Foglio1!D109</f>
-        <v>2970</v>
+        <v>19584</v>
       </c>
       <c r="E37" s="26"/>
       <c r="F37">
         <f t="shared" si="1"/>
-        <v>62900</v>
+        <v>45857</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="20">
         <f>Foglio1!A38*Foglio1!A110</f>
-        <v>2208</v>
+        <v>35955</v>
       </c>
       <c r="B38" s="20">
         <f>Foglio1!B38*Foglio1!B110</f>
-        <v>7093</v>
+        <v>31752</v>
       </c>
       <c r="C38" s="20">
         <f>Foglio1!C38*Foglio1!C110</f>
-        <v>31020</v>
+        <v>20292</v>
       </c>
       <c r="D38" s="20">
         <f>Foglio1!D38*Foglio1!D110</f>
-        <v>810</v>
+        <v>19448</v>
       </c>
       <c r="E38" s="26"/>
       <c r="F38">
         <f t="shared" si="1"/>
-        <v>41131</v>
+        <v>107447</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="20">
         <f>Foglio1!A39*Foglio1!A111</f>
-        <v>57318</v>
+        <v>59961</v>
       </c>
       <c r="B39" s="20">
         <f>Foglio1!B39*Foglio1!B111</f>
-        <v>15210</v>
+        <v>19050</v>
       </c>
       <c r="C39" s="20">
         <f>Foglio1!C39*Foglio1!C111</f>
-        <v>3952</v>
+        <v>37996</v>
       </c>
       <c r="D39" s="20">
         <f>Foglio1!D39*Foglio1!D111</f>
-        <v>24192</v>
+        <v>3393</v>
       </c>
       <c r="E39" s="26"/>
       <c r="F39">
         <f t="shared" si="1"/>
-        <v>100672</v>
+        <v>120400</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="20">
         <f>Foglio1!A40*Foglio1!A112</f>
-        <v>9288</v>
+        <v>448</v>
       </c>
       <c r="B40" s="20">
         <f>Foglio1!B40*Foglio1!B112</f>
-        <v>22736</v>
+        <v>11685</v>
       </c>
       <c r="C40" s="20">
         <f>Foglio1!C40*Foglio1!C112</f>
-        <v>12441</v>
+        <v>1292</v>
       </c>
       <c r="D40" s="20">
         <f>Foglio1!D40*Foglio1!D112</f>
-        <v>15355</v>
+        <v>8030</v>
       </c>
       <c r="E40" s="26"/>
       <c r="F40">
         <f t="shared" si="1"/>
-        <v>59820</v>
+        <v>21455</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="19">
         <f>Foglio1!A41*Foglio1!A81</f>
-        <v>20460</v>
+        <v>29028</v>
       </c>
       <c r="B41" s="19">
         <f>Foglio1!B41*Foglio1!B81</f>
-        <v>5332</v>
+        <v>0</v>
       </c>
       <c r="C41" s="19">
         <f>Foglio1!C41*Foglio1!C81</f>
-        <v>37355</v>
+        <v>0</v>
       </c>
       <c r="D41" s="19">
         <f>Foglio1!D41*Foglio1!D81</f>
-        <v>4323</v>
+        <v>39123</v>
       </c>
       <c r="E41" s="27"/>
       <c r="F41" s="22">
         <f>SUM(A41:D41)</f>
-        <v>67470</v>
+        <v>68151</v>
       </c>
       <c r="G41" s="22">
         <f>F41+F46+F51+F56</f>
-        <v>266408</v>
+        <v>307981</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="19">
         <f>Foglio1!A42*Foglio1!A82</f>
-        <v>38115</v>
+        <v>3762</v>
       </c>
       <c r="B42" s="19">
         <f>Foglio1!B42*Foglio1!B82</f>
-        <v>7345</v>
+        <v>32804</v>
       </c>
       <c r="C42" s="19">
         <f>Foglio1!C42*Foglio1!C82</f>
-        <v>13112</v>
+        <v>4860</v>
       </c>
       <c r="D42" s="19">
         <f>Foglio1!D42*Foglio1!D82</f>
-        <v>768</v>
+        <v>2240</v>
       </c>
       <c r="E42" s="27"/>
       <c r="F42">
         <f t="shared" ref="F42:F60" si="3">SUM(A42:D42)</f>
-        <v>59340</v>
+        <v>43666</v>
       </c>
       <c r="G42">
         <f t="shared" ref="G42:G45" si="4">F42+F47+F52+F57</f>
-        <v>256273</v>
+        <v>221578</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="19">
         <f>Foglio1!A43*Foglio1!A83</f>
-        <v>47800</v>
+        <v>4212</v>
       </c>
       <c r="B43" s="19">
         <f>Foglio1!B43*Foglio1!B83</f>
-        <v>23328</v>
+        <v>2478</v>
       </c>
       <c r="C43" s="19">
         <f>Foglio1!C43*Foglio1!C83</f>
-        <v>1300</v>
+        <v>3638</v>
       </c>
       <c r="D43" s="19">
         <f>Foglio1!D43*Foglio1!D83</f>
-        <v>50160</v>
+        <v>4025</v>
       </c>
       <c r="E43" s="27"/>
       <c r="F43">
         <f t="shared" si="3"/>
-        <v>122588</v>
+        <v>14353</v>
       </c>
       <c r="G43">
         <f t="shared" si="4"/>
-        <v>254531</v>
+        <v>164699</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="19">
         <f>Foglio1!A44*Foglio1!A84</f>
-        <v>33567</v>
+        <v>34340</v>
       </c>
       <c r="B44" s="19">
         <f>Foglio1!B44*Foglio1!B84</f>
-        <v>6440</v>
+        <v>16598</v>
       </c>
       <c r="C44" s="19">
         <f>Foglio1!C44*Foglio1!C84</f>
-        <v>1708</v>
+        <v>23766</v>
       </c>
       <c r="D44" s="19">
         <f>Foglio1!D44*Foglio1!D84</f>
-        <v>13340</v>
+        <v>8668</v>
       </c>
       <c r="E44" s="27"/>
       <c r="F44">
         <f t="shared" si="3"/>
-        <v>55055</v>
+        <v>83372</v>
       </c>
       <c r="G44">
         <f t="shared" si="4"/>
-        <v>312754</v>
+        <v>292028</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="19">
         <f>Foglio1!A45*Foglio1!A85</f>
-        <v>6765</v>
+        <v>17199</v>
       </c>
       <c r="B45" s="19">
         <f>Foglio1!B45*Foglio1!B85</f>
-        <v>7910</v>
+        <v>8480</v>
       </c>
       <c r="C45" s="19">
         <f>Foglio1!C45*Foglio1!C85</f>
-        <v>21228</v>
+        <v>33673</v>
       </c>
       <c r="D45" s="19">
         <f>Foglio1!D45*Foglio1!D85</f>
-        <v>4640</v>
+        <v>4320</v>
       </c>
       <c r="E45" s="27"/>
       <c r="F45">
         <f t="shared" si="3"/>
-        <v>40543</v>
+        <v>63672</v>
       </c>
       <c r="G45">
         <f t="shared" si="4"/>
-        <v>241423</v>
+        <v>211970</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="20">
         <f>Foglio1!A90*Foglio1!A46</f>
-        <v>31320</v>
+        <v>27412</v>
       </c>
       <c r="B46" s="20">
         <f>Foglio1!B90*Foglio1!B46</f>
-        <v>11970</v>
+        <v>19402</v>
       </c>
       <c r="C46" s="20">
         <f>Foglio1!C90*Foglio1!C46</f>
-        <v>17640</v>
+        <v>3762</v>
       </c>
       <c r="D46" s="20">
         <f>Foglio1!D90*Foglio1!D46</f>
-        <v>4590</v>
+        <v>2475</v>
       </c>
       <c r="E46" s="27"/>
       <c r="F46">
         <f t="shared" si="3"/>
-        <v>65520</v>
+        <v>53051</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="20">
         <f>Foglio1!A91*Foglio1!A47</f>
-        <v>11449</v>
+        <v>8843</v>
       </c>
       <c r="B47" s="20">
         <f>Foglio1!B91*Foglio1!B47</f>
-        <v>19591</v>
+        <v>10556</v>
       </c>
       <c r="C47" s="20">
         <f>Foglio1!C91*Foglio1!C47</f>
-        <v>8075</v>
+        <v>18144</v>
       </c>
       <c r="D47" s="20">
         <f>Foglio1!D91*Foglio1!D47</f>
-        <v>20736</v>
+        <v>19800</v>
       </c>
       <c r="E47" s="27"/>
       <c r="F47">
         <f t="shared" si="3"/>
-        <v>59851</v>
+        <v>57343</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="20">
         <f>Foglio1!A92*Foglio1!A48</f>
-        <v>22088</v>
+        <v>2303</v>
       </c>
       <c r="B48" s="20">
         <f>Foglio1!B92*Foglio1!B48</f>
-        <v>2534</v>
+        <v>20790</v>
       </c>
       <c r="C48" s="20">
         <f>Foglio1!C92*Foglio1!C48</f>
-        <v>1825</v>
+        <v>1536</v>
       </c>
       <c r="D48" s="20">
         <f>Foglio1!D92*Foglio1!D48</f>
-        <v>7788</v>
+        <v>3795</v>
       </c>
       <c r="E48" s="27"/>
       <c r="F48">
         <f t="shared" si="3"/>
-        <v>34235</v>
+        <v>28424</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="20">
         <f>Foglio1!A93*Foglio1!A49</f>
-        <v>1892</v>
+        <v>29415</v>
       </c>
       <c r="B49" s="20">
         <f>Foglio1!B93*Foglio1!B49</f>
-        <v>18512</v>
+        <v>2460</v>
       </c>
       <c r="C49" s="20">
         <f>Foglio1!C93*Foglio1!C49</f>
-        <v>56105</v>
+        <v>6384</v>
       </c>
       <c r="D49" s="20">
         <f>Foglio1!D93*Foglio1!D49</f>
-        <v>1003</v>
+        <v>29725</v>
       </c>
       <c r="E49" s="27"/>
       <c r="F49">
         <f t="shared" si="3"/>
-        <v>77512</v>
+        <v>67984</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="20">
         <f>Foglio1!A94*Foglio1!A50</f>
-        <v>845</v>
+        <v>17880</v>
       </c>
       <c r="B50" s="20">
         <f>Foglio1!B94*Foglio1!B50</f>
-        <v>172</v>
+        <v>0</v>
       </c>
       <c r="C50" s="20">
         <f>Foglio1!C94*Foglio1!C50</f>
-        <v>27467</v>
+        <v>41829</v>
       </c>
       <c r="D50" s="20">
         <f>Foglio1!D94*Foglio1!D50</f>
-        <v>48178</v>
+        <v>27811</v>
       </c>
       <c r="E50" s="27"/>
       <c r="F50">
         <f t="shared" si="3"/>
-        <v>76662</v>
+        <v>87520</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="19">
         <f>Foglio1!A51*Foglio1!A99</f>
-        <v>23184</v>
+        <v>21200</v>
       </c>
       <c r="B51" s="19">
         <f>Foglio1!B51*Foglio1!B99</f>
-        <v>37249</v>
+        <v>17064</v>
       </c>
       <c r="C51" s="19">
         <f>Foglio1!C51*Foglio1!C99</f>
-        <v>5652</v>
+        <v>38760</v>
       </c>
       <c r="D51" s="19">
         <f>Foglio1!D51*Foglio1!D99</f>
-        <v>34884</v>
+        <v>9890</v>
       </c>
       <c r="E51" s="27"/>
       <c r="F51">
         <f t="shared" si="3"/>
-        <v>100969</v>
+        <v>86914</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="19">
         <f>Foglio1!A52*Foglio1!A100</f>
-        <v>32580</v>
+        <v>16380</v>
       </c>
       <c r="B52" s="19">
         <f>Foglio1!B52*Foglio1!B100</f>
-        <v>72</v>
+        <v>165</v>
       </c>
       <c r="C52" s="19">
         <f>Foglio1!C52*Foglio1!C100</f>
-        <v>11259</v>
+        <v>15330</v>
       </c>
       <c r="D52" s="19">
         <f>Foglio1!D52*Foglio1!D100</f>
-        <v>4848</v>
+        <v>2130</v>
       </c>
       <c r="E52" s="27"/>
       <c r="F52">
         <f t="shared" si="3"/>
-        <v>48759</v>
+        <v>34005</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="19">
         <f>Foglio1!A53*Foglio1!A101</f>
-        <v>1330</v>
+        <v>10488</v>
       </c>
       <c r="B53" s="19">
         <f>Foglio1!B53*Foglio1!B101</f>
-        <v>4628</v>
+        <v>1610</v>
       </c>
       <c r="C53" s="19">
         <f>Foglio1!C53*Foglio1!C101</f>
-        <v>2726</v>
+        <v>16940</v>
       </c>
       <c r="D53" s="19">
         <f>Foglio1!D53*Foglio1!D101</f>
-        <v>36288</v>
+        <v>5522</v>
       </c>
       <c r="E53" s="27"/>
       <c r="F53">
         <f t="shared" si="3"/>
-        <v>44972</v>
+        <v>34560</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="19">
         <f>Foglio1!A54*Foglio1!A102</f>
-        <v>3276</v>
+        <v>2394</v>
       </c>
       <c r="B54" s="19">
         <f>Foglio1!B54*Foglio1!B102</f>
-        <v>47092</v>
+        <v>6512</v>
       </c>
       <c r="C54" s="19">
         <f>Foglio1!C54*Foglio1!C102</f>
-        <v>48880</v>
+        <v>8468</v>
       </c>
       <c r="D54" s="19">
         <f>Foglio1!D54*Foglio1!D102</f>
-        <v>4508</v>
+        <v>1926</v>
       </c>
       <c r="E54" s="27"/>
       <c r="F54">
         <f t="shared" si="3"/>
-        <v>103756</v>
+        <v>19300</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="19">
         <f>Foglio1!A55*Foglio1!A103</f>
-        <v>29868</v>
+        <v>10275</v>
       </c>
       <c r="B55" s="19">
         <f>Foglio1!B55*Foglio1!B103</f>
-        <v>9617</v>
+        <v>3900</v>
       </c>
       <c r="C55" s="19">
         <f>Foglio1!C55*Foglio1!C103</f>
-        <v>26296</v>
+        <v>24881</v>
       </c>
       <c r="D55" s="19">
         <f>Foglio1!D55*Foglio1!D103</f>
-        <v>22372</v>
+        <v>528</v>
       </c>
       <c r="E55" s="27"/>
       <c r="F55">
         <f t="shared" si="3"/>
-        <v>88153</v>
+        <v>39584</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="20">
         <f>Foglio1!A56*Foglio1!A108</f>
-        <v>1836</v>
+        <v>42639</v>
       </c>
       <c r="B56" s="20">
         <f>Foglio1!B56*Foglio1!B108</f>
-        <v>54</v>
+        <v>28296</v>
       </c>
       <c r="C56" s="20">
         <f>Foglio1!C56*Foglio1!C108</f>
-        <v>17850</v>
+        <v>20812</v>
       </c>
       <c r="D56" s="20">
         <f>Foglio1!D56*Foglio1!D108</f>
-        <v>12709</v>
+        <v>8118</v>
       </c>
       <c r="E56" s="27"/>
       <c r="F56">
         <f t="shared" si="3"/>
-        <v>32449</v>
+        <v>99865</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="20">
         <f>Foglio1!A57*Foglio1!A109</f>
-        <v>42120</v>
+        <v>4104</v>
       </c>
       <c r="B57" s="20">
         <f>Foglio1!B57*Foglio1!B109</f>
-        <v>19950</v>
+        <v>27370</v>
       </c>
       <c r="C57" s="20">
         <f>Foglio1!C57*Foglio1!C109</f>
-        <v>12483</v>
+        <v>37714</v>
       </c>
       <c r="D57" s="20">
         <f>Foglio1!D57*Foglio1!D109</f>
-        <v>13770</v>
+        <v>17376</v>
       </c>
       <c r="E57" s="27"/>
       <c r="F57">
         <f t="shared" si="3"/>
-        <v>88323</v>
+        <v>86564</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="20">
         <f>Foglio1!A58*Foglio1!A110</f>
-        <v>5704</v>
+        <v>34827</v>
       </c>
       <c r="B58" s="20">
         <f>Foglio1!B58*Foglio1!B110</f>
-        <v>27334</v>
+        <v>47376</v>
       </c>
       <c r="C58" s="20">
         <f>Foglio1!C58*Foglio1!C110</f>
-        <v>18048</v>
+        <v>4895</v>
       </c>
       <c r="D58" s="20">
         <f>Foglio1!D58*Foglio1!D110</f>
-        <v>1650</v>
+        <v>264</v>
       </c>
       <c r="E58" s="27"/>
       <c r="F58">
         <f t="shared" si="3"/>
-        <v>52736</v>
+        <v>87362</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="20">
         <f>Foglio1!A59*Foglio1!A111</f>
-        <v>12792</v>
+        <v>44022</v>
       </c>
       <c r="B59" s="20">
         <f>Foglio1!B59*Foglio1!B111</f>
-        <v>38220</v>
+        <v>39116</v>
       </c>
       <c r="C59" s="20">
         <f>Foglio1!C59*Foglio1!C111</f>
-        <v>2907</v>
+        <v>34928</v>
       </c>
       <c r="D59" s="20">
         <f>Foglio1!D59*Foglio1!D111</f>
-        <v>22512</v>
+        <v>3306</v>
       </c>
       <c r="E59" s="27"/>
       <c r="F59">
         <f t="shared" si="3"/>
-        <v>76431</v>
+        <v>121372</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="20">
         <f>Foglio1!A60*Foglio1!A112</f>
-        <v>2304</v>
+        <v>448</v>
       </c>
       <c r="B60" s="20">
         <f>Foglio1!B60*Foglio1!B112</f>
-        <v>13456</v>
+        <v>11628</v>
       </c>
       <c r="C60" s="20">
         <f>Foglio1!C60*Foglio1!C112</f>
-        <v>2958</v>
+        <v>4446</v>
       </c>
       <c r="D60" s="20">
         <f>Foglio1!D60*Foglio1!D112</f>
-        <v>17347</v>
+        <v>4672</v>
       </c>
       <c r="E60" s="27"/>
       <c r="F60">
         <f t="shared" si="3"/>
-        <v>36065</v>
+        <v>21194</v>
       </c>
     </row>
   </sheetData>
@@ -4093,545 +4093,545 @@
     <row r="1" spans="1:11">
       <c r="A1" s="19">
         <f>Foglio1!A1*Foglio1!A82</f>
-        <v>13200</v>
+        <v>2628</v>
       </c>
       <c r="B1" s="19">
         <f>Foglio1!B1*Foglio1!B82</f>
-        <v>13673</v>
+        <v>14868</v>
       </c>
       <c r="C1" s="19">
         <f>Foglio1!C1*Foglio1!C82</f>
-        <v>35462</v>
+        <v>24408</v>
       </c>
       <c r="D1" s="19">
         <f>Foglio1!D1*Foglio1!D82</f>
-        <v>14080</v>
+        <v>24864</v>
       </c>
       <c r="E1" s="26"/>
       <c r="F1">
         <f>SUM(A1:D1)</f>
-        <v>76415</v>
+        <v>66768</v>
       </c>
       <c r="G1">
         <f>F1+F6+F11+F16</f>
-        <v>277799</v>
+        <v>285122</v>
       </c>
       <c r="H1">
         <f>SUM(A1:A5)</f>
-        <v>74494</v>
+        <v>111307</v>
       </c>
       <c r="I1">
         <f t="shared" ref="I1:K1" si="0">SUM(B1:B5)</f>
-        <v>113892</v>
+        <v>101212</v>
       </c>
       <c r="J1">
         <f t="shared" si="0"/>
-        <v>86445</v>
+        <v>92146</v>
       </c>
       <c r="K1">
         <f t="shared" si="0"/>
-        <v>57430</v>
+        <v>46247</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="19">
         <f>Foglio1!A2*Foglio1!A83</f>
-        <v>19837</v>
+        <v>5346</v>
       </c>
       <c r="B2" s="19">
         <f>Foglio1!B2*Foglio1!B83</f>
-        <v>52731</v>
+        <v>11918</v>
       </c>
       <c r="C2" s="19">
         <f>Foglio1!C2*Foglio1!C83</f>
-        <v>6275</v>
+        <v>11556</v>
       </c>
       <c r="D2" s="19">
         <f>Foglio1!D2*Foglio1!D83</f>
-        <v>2400</v>
+        <v>6350</v>
       </c>
       <c r="E2" s="26"/>
       <c r="F2">
         <f t="shared" ref="F2:F20" si="1">SUM(A2:D2)</f>
-        <v>81243</v>
+        <v>35170</v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G5" si="2">F2+F7+F12+F17</f>
-        <v>219252</v>
+        <v>206632</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="19">
         <f>Foglio1!A3*Foglio1!A84</f>
-        <v>8350</v>
+        <v>36158</v>
       </c>
       <c r="B3" s="19">
         <f>Foglio1!B3*Foglio1!B84</f>
-        <v>6020</v>
+        <v>12728</v>
       </c>
       <c r="C3" s="19">
         <f>Foglio1!C3*Foglio1!C84</f>
-        <v>2996</v>
+        <v>24072</v>
       </c>
       <c r="D3" s="19">
         <f>Foglio1!D3*Foglio1!D84</f>
-        <v>15088</v>
+        <v>7172</v>
       </c>
       <c r="E3" s="26"/>
       <c r="F3">
         <f t="shared" si="1"/>
-        <v>32454</v>
+        <v>80130</v>
       </c>
       <c r="G3">
         <f t="shared" si="2"/>
-        <v>218778</v>
+        <v>312319</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="19">
         <f>Foglio1!A4*Foglio1!A85</f>
-        <v>1760</v>
+        <v>26838</v>
       </c>
       <c r="B4" s="19">
         <f>Foglio1!B4*Foglio1!B85</f>
-        <v>22826</v>
+        <v>23426</v>
       </c>
       <c r="C4" s="19">
         <f>Foglio1!C4*Foglio1!C85</f>
-        <v>15834</v>
+        <v>24160</v>
       </c>
       <c r="D4" s="19">
         <f>Foglio1!D4*Foglio1!D85</f>
-        <v>448</v>
+        <v>7830</v>
       </c>
       <c r="E4" s="26"/>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>40868</v>
+        <v>82254</v>
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
-        <v>171107</v>
+        <v>196012</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="19">
         <f>Foglio1!A5*Foglio1!A86</f>
-        <v>31347</v>
+        <v>40337</v>
       </c>
       <c r="B5" s="19">
         <f>Foglio1!B5*Foglio1!B86</f>
-        <v>18642</v>
+        <v>38272</v>
       </c>
       <c r="C5" s="19">
         <f>Foglio1!C5*Foglio1!C86</f>
-        <v>25878</v>
+        <v>7950</v>
       </c>
       <c r="D5" s="19">
         <f>Foglio1!D5*Foglio1!D86</f>
-        <v>25414</v>
+        <v>31</v>
       </c>
       <c r="E5" s="26"/>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>101281</v>
+        <v>86590</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>315518</v>
+        <v>216826</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="20">
         <f>Foglio1!A6*Foglio1!A91</f>
-        <v>1926</v>
+        <v>45649</v>
       </c>
       <c r="B6" s="20">
         <f>Foglio1!B6*Foglio1!B91</f>
-        <v>36465</v>
+        <v>4640</v>
       </c>
       <c r="C6" s="20">
         <f>Foglio1!C6*Foglio1!C91</f>
-        <v>765</v>
+        <v>49140</v>
       </c>
       <c r="D6" s="20">
         <f>Foglio1!D6*Foglio1!D91</f>
-        <v>41904</v>
+        <v>19140</v>
       </c>
       <c r="E6" s="26"/>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>81060</v>
+        <v>118569</v>
       </c>
       <c r="H6">
         <f>SUM(A6:A10)</f>
-        <v>47517</v>
+        <v>93996</v>
       </c>
       <c r="I6">
         <f t="shared" ref="I6" si="3">SUM(B6:B10)</f>
-        <v>91842</v>
+        <v>64472</v>
       </c>
       <c r="J6">
         <f t="shared" ref="J6" si="4">SUM(C6:C10)</f>
-        <v>101332</v>
+        <v>59270</v>
       </c>
       <c r="K6">
         <f t="shared" ref="K6" si="5">SUM(D6:D10)</f>
-        <v>102844</v>
+        <v>101516</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="20">
         <f>Foglio1!A7*Foglio1!A92</f>
-        <v>11968</v>
+        <v>8232</v>
       </c>
       <c r="B7" s="20">
         <f>Foglio1!B7*Foglio1!B92</f>
-        <v>168</v>
+        <v>18144</v>
       </c>
       <c r="C7" s="20">
         <f>Foglio1!C7*Foglio1!C92</f>
-        <v>12337</v>
+        <v>1008</v>
       </c>
       <c r="D7" s="20">
         <f>Foglio1!D7*Foglio1!D92</f>
-        <v>11550</v>
+        <v>15456</v>
       </c>
       <c r="E7" s="26"/>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>36023</v>
+        <v>42840</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="20">
         <f>Foglio1!A8*Foglio1!A93</f>
-        <v>1936</v>
+        <v>34225</v>
       </c>
       <c r="B8" s="20">
         <f>Foglio1!B8*Foglio1!B93</f>
-        <v>25688</v>
+        <v>3321</v>
       </c>
       <c r="C8" s="20">
         <f>Foglio1!C8*Foglio1!C93</f>
-        <v>54880</v>
+        <v>3472</v>
       </c>
       <c r="D8" s="20">
         <f>Foglio1!D8*Foglio1!D93</f>
-        <v>3481</v>
+        <v>25085</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>85985</v>
+        <v>66103</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="20">
         <f>Foglio1!A9*Foglio1!A94</f>
-        <v>15925</v>
+        <v>2980</v>
       </c>
       <c r="B9" s="20">
         <f>Foglio1!B9*Foglio1!B94</f>
-        <v>8815</v>
+        <v>0</v>
       </c>
       <c r="C9" s="20">
         <f>Foglio1!C9*Foglio1!C94</f>
-        <v>8591</v>
+        <v>2292</v>
       </c>
       <c r="D9" s="20">
         <f>Foglio1!D9*Foglio1!D94</f>
-        <v>44421</v>
+        <v>34387</v>
       </c>
       <c r="E9" s="26"/>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>77752</v>
+        <v>39659</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="20">
         <f>Foglio1!A10*Foglio1!A95</f>
-        <v>15762</v>
+        <v>2910</v>
       </c>
       <c r="B10" s="20">
         <f>Foglio1!B10*Foglio1!B95</f>
-        <v>20706</v>
+        <v>38367</v>
       </c>
       <c r="C10" s="20">
         <f>Foglio1!C10*Foglio1!C95</f>
-        <v>24759</v>
+        <v>3358</v>
       </c>
       <c r="D10" s="20">
         <f>Foglio1!D10*Foglio1!D95</f>
-        <v>1488</v>
+        <v>7448</v>
       </c>
       <c r="E10" s="26"/>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>62715</v>
+        <v>52083</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="19">
         <f>Foglio1!A11*Foglio1!A100</f>
-        <v>35838</v>
+        <v>15210</v>
       </c>
       <c r="B11" s="19">
         <f>Foglio1!B11*Foglio1!B100</f>
-        <v>60</v>
+        <v>1364</v>
       </c>
       <c r="C11" s="19">
         <f>Foglio1!C11*Foglio1!C100</f>
-        <v>34889</v>
+        <v>24045</v>
       </c>
       <c r="D11" s="19">
         <f>Foglio1!D11*Foglio1!D100</f>
-        <v>2112</v>
+        <v>13206</v>
       </c>
       <c r="E11" s="26"/>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>72899</v>
+        <v>53825</v>
       </c>
       <c r="H11">
         <f>SUM(A11:A15)</f>
-        <v>75441</v>
+        <v>120797</v>
       </c>
       <c r="I11">
         <f t="shared" ref="I11" si="6">SUM(B11:B15)</f>
-        <v>74914</v>
+        <v>29890</v>
       </c>
       <c r="J11">
         <f t="shared" ref="J11" si="7">SUM(C11:C15)</f>
-        <v>78224</v>
+        <v>65552</v>
       </c>
       <c r="K11">
         <f t="shared" ref="K11" si="8">SUM(D11:D15)</f>
-        <v>52664</v>
+        <v>27173</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="19">
         <f>Foglio1!A12*Foglio1!A101</f>
-        <v>6090</v>
+        <v>25194</v>
       </c>
       <c r="B12" s="19">
         <f>Foglio1!B12*Foglio1!B101</f>
-        <v>2759</v>
+        <v>3864</v>
       </c>
       <c r="C12" s="19">
         <f>Foglio1!C12*Foglio1!C101</f>
-        <v>12220</v>
+        <v>10406</v>
       </c>
       <c r="D12" s="19">
         <f>Foglio1!D12*Foglio1!D101</f>
-        <v>33600</v>
+        <v>1100</v>
       </c>
       <c r="E12" s="26"/>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>54669</v>
+        <v>40564</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="19">
         <f>Foglio1!A13*Foglio1!A102</f>
-        <v>2613</v>
+        <v>26334</v>
       </c>
       <c r="B13" s="19">
         <f>Foglio1!B13*Foglio1!B102</f>
-        <v>27985</v>
+        <v>10138</v>
       </c>
       <c r="C13" s="19">
         <f>Foglio1!C13*Foglio1!C102</f>
-        <v>3290</v>
+        <v>10147</v>
       </c>
       <c r="D13" s="19">
         <f>Foglio1!D13*Foglio1!D102</f>
-        <v>12936</v>
+        <v>2124</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>46824</v>
+        <v>48743</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="19">
         <f>Foglio1!A14*Foglio1!A103</f>
-        <v>4104</v>
+        <v>18150</v>
       </c>
       <c r="B14" s="19">
         <f>Foglio1!B14*Foglio1!B103</f>
-        <v>11682</v>
+        <v>3100</v>
       </c>
       <c r="C14" s="19">
         <f>Foglio1!C14*Foglio1!C103</f>
-        <v>11248</v>
+        <v>19869</v>
       </c>
       <c r="D14" s="19">
         <f>Foglio1!D14*Foglio1!D103</f>
-        <v>3196</v>
+        <v>8151</v>
       </c>
       <c r="E14" s="26"/>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>30230</v>
+        <v>49270</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="19">
         <f>Foglio1!A15*Foglio1!A104</f>
-        <v>26796</v>
+        <v>35909</v>
       </c>
       <c r="B15" s="19">
         <f>Foglio1!B15*Foglio1!B104</f>
-        <v>32428</v>
+        <v>11424</v>
       </c>
       <c r="C15" s="19">
         <f>Foglio1!C15*Foglio1!C104</f>
-        <v>16577</v>
+        <v>1085</v>
       </c>
       <c r="D15" s="19">
         <f>Foglio1!D15*Foglio1!D104</f>
-        <v>820</v>
+        <v>2592</v>
       </c>
       <c r="E15" s="26"/>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>76621</v>
+        <v>51010</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="20">
         <f>Foglio1!A16*Foglio1!A109</f>
-        <v>13500</v>
+        <v>2430</v>
       </c>
       <c r="B16" s="20">
         <f>Foglio1!B16*Foglio1!B109</f>
-        <v>14700</v>
+        <v>33350</v>
       </c>
       <c r="C16" s="20">
         <f>Foglio1!C16*Foglio1!C109</f>
-        <v>6643</v>
+        <v>5668</v>
       </c>
       <c r="D16" s="20">
         <f>Foglio1!D16*Foglio1!D109</f>
-        <v>12582</v>
+        <v>4512</v>
       </c>
       <c r="E16" s="26"/>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>47425</v>
+        <v>45960</v>
       </c>
       <c r="H16">
         <f>SUM(A16:A20)</f>
-        <v>83647</v>
+        <v>73532</v>
       </c>
       <c r="I16">
         <f t="shared" ref="I16" si="9">SUM(B16:B20)</f>
-        <v>96557</v>
+        <v>112693</v>
       </c>
       <c r="J16">
         <f t="shared" ref="J16" si="10">SUM(C16:C20)</f>
-        <v>24466</v>
+        <v>66422</v>
       </c>
       <c r="K16">
         <f t="shared" ref="K16" si="11">SUM(D16:D20)</f>
-        <v>40745</v>
+        <v>50686</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="20">
         <f>Foglio1!A17*Foglio1!A110</f>
-        <v>2116</v>
+        <v>14946</v>
       </c>
       <c r="B17" s="20">
         <f>Foglio1!B17*Foglio1!B110</f>
-        <v>31832</v>
+        <v>47628</v>
       </c>
       <c r="C17" s="20">
         <f>Foglio1!C17*Foglio1!C110</f>
-        <v>11139</v>
+        <v>4628</v>
       </c>
       <c r="D17" s="20">
         <f>Foglio1!D17*Foglio1!D110</f>
-        <v>2230</v>
+        <v>20856</v>
       </c>
       <c r="E17" s="26"/>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>47317</v>
+        <v>88058</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="20">
         <f>Foglio1!A18*Foglio1!A111</f>
-        <v>46986</v>
+        <v>52118</v>
       </c>
       <c r="B18" s="20">
         <f>Foglio1!B18*Foglio1!B111</f>
-        <v>1170</v>
+        <v>23622</v>
       </c>
       <c r="C18" s="20">
         <f>Foglio1!C18*Foglio1!C111</f>
-        <v>95</v>
+        <v>33512</v>
       </c>
       <c r="D18" s="20">
         <f>Foglio1!D18*Foglio1!D111</f>
-        <v>5264</v>
+        <v>8091</v>
       </c>
       <c r="E18" s="26"/>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>53515</v>
+        <v>117343</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="20">
         <f>Foglio1!A19*Foglio1!A112</f>
-        <v>5112</v>
+        <v>3968</v>
       </c>
       <c r="B19" s="20">
         <f>Foglio1!B19*Foglio1!B112</f>
-        <v>2320</v>
+        <v>285</v>
       </c>
       <c r="C19" s="20">
         <f>Foglio1!C19*Foglio1!C112</f>
-        <v>6525</v>
+        <v>7144</v>
       </c>
       <c r="D19" s="20">
         <f>Foglio1!D19*Foglio1!D112</f>
-        <v>8300</v>
+        <v>13432</v>
       </c>
       <c r="E19" s="26"/>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>22257</v>
+        <v>24829</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="20">
         <f>Foglio1!A20*Foglio1!A113</f>
-        <v>15933</v>
+        <v>70</v>
       </c>
       <c r="B20" s="20">
         <f>Foglio1!B20*Foglio1!B113</f>
-        <v>46535</v>
+        <v>7808</v>
       </c>
       <c r="C20" s="20">
         <f>Foglio1!C20*Foglio1!C113</f>
-        <v>64</v>
+        <v>15470</v>
       </c>
       <c r="D20" s="20">
         <f>Foglio1!D20*Foglio1!D113</f>
-        <v>12369</v>
+        <v>3795</v>
       </c>
       <c r="E20" s="26"/>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>74901</v>
+        <v>27143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>